<commit_message>
Force push latest save script and updates
</commit_message>
<xml_diff>
--- a/database/players_filled.xlsx
+++ b/database/players_filled.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AC10"/>
+  <dimension ref="A1:AC47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -590,43 +590,41 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Jordie </t>
+          <t>Andrew</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Barrett</t>
+          <t>Porter</t>
         </is>
       </c>
       <c r="D2" s="2" t="n">
-        <v>34700</v>
+        <v>32874</v>
       </c>
       <c r="E2" t="n">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="F2" t="n">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="G2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H2" t="n">
-        <v>97.39166666666667</v>
-      </c>
-      <c r="I2" t="n">
-        <v>13</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr"/>
       <c r="N2" t="inlineStr">
         <is>
-          <t>ct:5,wg:5,fb:4,FH:3</t>
+          <t>lp:5</t>
         </is>
       </c>
       <c r="O2" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="P2" t="inlineStr"/>
       <c r="Q2" t="inlineStr"/>
@@ -644,12 +642,12 @@
       <c r="AA2" t="inlineStr"/>
       <c r="AB2" t="inlineStr">
         <is>
-          <t>{"darts": 5.0, "finishing": 9.0, "footwork": 7.0, "goal_kicking": 19.0, "handling": 16.0, "kicking": 18.0, "kicking_power": 20.0, "lineouts": 10.0, "marking": 14.0, "offloading": 5.0, "passing": 19.0, "scrummaging": 10.0, "rucking": 12.0, "technique": 15.0, "aggression": 18.0, "anticipation": 20.0, "bravery": 7.0, "composure": 19.0, "concentration": 13.0, "decisions": 17.0, "determination": 6.0, "flair": 20.0, "leadership": 13.0, "off_the_ball": 13.0, "positioning": 6.0, "teamwork": 7.0, "vision": 20.0, "work_rate": 9.0, "acceleration": 9.0, "agility": 14.0, "balance": 20.0, "jumping_reach": 9.0, "natural_fitness": 20.0, "pace": 9.0, "stamina": 20.0, "strength": 17.0}</t>
+          <t>{"darts": 4.0, "finishing": 5.0, "footwork": 9.0, "goal_kicking": 5.0, "handling": 6.0, "kicking": 5.0, "kicking_power": 5.0, "lineouts": 2.0, "marking": 20.0, "offloading": 5.0, "passing": 13.0, "scrummaging": 16.0, "rucking": 19.0, "technique": 9.0, "aggression": 8.0, "anticipation": 9.0, "bravery": 10.0, "composure": 15.0, "concentration": 16.0, "decisions": 19.0, "determination": 11.0, "flair": 14.0, "leadership": 13.0, "off_the_ball": 10.0, "positioning": 7.0, "teamwork": 9.0, "vision": 16.0, "work_rate": 4.0, "acceleration": 12.0, "agility": 3.0, "balance": 12.0, "jumping_reach": 5.0, "natural_fitness": 13.0, "pace": 11.0, "stamina": 11.0, "strength": 16.0}</t>
         </is>
       </c>
       <c r="AC2" t="inlineStr">
         <is>
-          <t>{"Consistency": 14.7, "Controversy": 1.0, "Dirtiness": 3.8, "Important Matches": 15.5, "Injury Proneness": 10.8, "Loyalty": 14.8, "Pressure": 19.0, "Professionalism": 19.0, "Sportsmanship": 17.9, "Temperament": 17.8, "Versatility": 14.2, "Ambition": 17.4, "Adaptability": 18.7}</t>
+          <t>{"Consistency": 18.5, "Controversy": 3.6, "Dirtiness": 4.1, "Important Matches": 16.0, "Injury Proneness": 9.1, "Loyalty": 15.0, "Pressure": 17.9, "Professionalism": 19.4, "Sportsmanship": 17.3, "Temperament": 19.0, "Versatility": 14.8, "Ambition": 19.6, "Adaptability": 18.5}</t>
         </is>
       </c>
     </row>
@@ -659,43 +657,41 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t xml:space="preserve">James </t>
+          <t>Dan</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Ryan</t>
+          <t>Sheehan</t>
         </is>
       </c>
       <c r="D3" s="2" t="n">
-        <v>34732</v>
+        <v>32875</v>
       </c>
       <c r="E3" t="n">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="F3" t="n">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="G3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H3" t="n">
-        <v>86.52499999999999</v>
-      </c>
-      <c r="I3" t="n">
-        <v>2</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="I3" t="inlineStr"/>
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr"/>
       <c r="M3" t="inlineStr"/>
       <c r="N3" t="inlineStr">
         <is>
-          <t>sr:5, br:2</t>
+          <t>hk:5</t>
         </is>
       </c>
       <c r="O3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P3" t="inlineStr"/>
       <c r="Q3" t="inlineStr"/>
@@ -706,19 +702,19 @@
       <c r="V3" t="inlineStr"/>
       <c r="W3" t="inlineStr"/>
       <c r="X3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Y3" t="inlineStr"/>
       <c r="Z3" t="inlineStr"/>
       <c r="AA3" t="inlineStr"/>
       <c r="AB3" t="inlineStr">
         <is>
-          <t>{"darts": 4.0, "finishing": 5.0, "footwork": 18.0, "goal_kicking": 5.0, "handling": 18.0, "kicking": 6.0, "kicking_power": 6.0, "lineouts": 17.0, "marking": 6.0, "offloading": 6.0, "passing": 9.0, "scrummaging": 20.0, "rucking": 4.0, "technique": 5.0, "aggression": 8.0, "anticipation": 19.0, "bravery": 6.0, "composure": 11.0, "concentration": 12.0, "decisions": 18.0, "determination": 13.0, "flair": 7.0, "leadership": 12.0, "off_the_ball": 10.0, "positioning": 15.0, "teamwork": 13.0, "vision": 16.0, "work_rate": 13.0, "acceleration": 19.0, "agility": 8.0, "balance": 8.0, "jumping_reach": 8.0, "natural_fitness": 19.0, "pace": 17.0, "stamina": 20.0, "strength": 15.0}</t>
+          <t>{"darts": 5.0, "finishing": 8.0, "footwork": 2.0, "goal_kicking": 1.0, "handling": 11.0, "kicking": 10.0, "kicking_power": 5.0, "lineouts": 9.0, "marking": 13.0, "offloading": 13.0, "passing": 20.0, "scrummaging": 18.0, "rucking": 9.0, "technique": 2.0, "aggression": 12.0, "anticipation": 17.0, "bravery": 19.0, "composure": 13.0, "concentration": 17.0, "decisions": 6.0, "determination": 7.0, "flair": 17.0, "leadership": 8.0, "off_the_ball": 2.0, "positioning": 12.0, "teamwork": 2.0, "vision": 8.0, "work_rate": 9.0, "acceleration": 10.0, "agility": 10.0, "balance": 11.0, "jumping_reach": 9.0, "natural_fitness": 17.0, "pace": 5.0, "stamina": 18.0, "strength": 9.0}</t>
         </is>
       </c>
       <c r="AC3" t="inlineStr">
         <is>
-          <t>{"Consistency": 18.7, "Controversy": 3.5, "Dirtiness": 18.0, "Important Matches": 14.6, "Injury Proneness": 16.3, "Loyalty": 3.8, "Pressure": 15.7, "Professionalism": 18.4, "Sportsmanship": 3.9, "Temperament": 8.4, "Versatility": 11.4, "Ambition": 16.9, "Adaptability": 17.4}</t>
+          <t>{"Consistency": 17.5, "Controversy": 4.0, "Dirtiness": 1.5, "Important Matches": 19.1, "Injury Proneness": 7.6, "Loyalty": 18.6, "Pressure": 17.9, "Professionalism": 19.4, "Sportsmanship": 17.9, "Temperament": 19.2, "Versatility": 1.9, "Ambition": 17.6, "Adaptability": 17.0}</t>
         </is>
       </c>
     </row>
@@ -728,43 +724,41 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Joe </t>
+          <t xml:space="preserve">Tadgh </t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>McCarthy</t>
+          <t>Furlong</t>
         </is>
       </c>
       <c r="D4" s="2" t="n">
-        <v>34733</v>
+        <v>32876</v>
       </c>
       <c r="E4" t="n">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="F4" t="n">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="G4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H4" t="n">
-        <v>84.99166666666666</v>
-      </c>
-      <c r="I4" t="n">
-        <v>2</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr"/>
       <c r="M4" t="inlineStr"/>
       <c r="N4" t="inlineStr">
         <is>
-          <t>sr:5, br:3</t>
+          <t>tp:5</t>
         </is>
       </c>
       <c r="O4" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="P4" t="inlineStr"/>
       <c r="Q4" t="inlineStr"/>
@@ -775,19 +769,19 @@
       <c r="V4" t="inlineStr"/>
       <c r="W4" t="inlineStr"/>
       <c r="X4" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="Y4" t="inlineStr"/>
       <c r="Z4" t="inlineStr"/>
       <c r="AA4" t="inlineStr"/>
       <c r="AB4" t="inlineStr">
         <is>
-          <t>{"darts": 5.0, "finishing": 5.0, "footwork": 8.0, "goal_kicking": 5.0, "handling": 4.0, "kicking": 6.0, "kicking_power": 5.0, "lineouts": 9.0, "marking": 10.0, "offloading": 9.0, "passing": 19.0, "scrummaging": 20.0, "rucking": 9.0, "technique": 12.0, "aggression": 4.0, "anticipation": 7.0, "bravery": 4.0, "composure": 20.0, "concentration": 20.0, "decisions": 20.0, "determination": 10.0, "flair": 6.0, "leadership": 19.0, "off_the_ball": 11.0, "positioning": 11.0, "teamwork": 15.0, "vision": 16.0, "work_rate": 20.0, "acceleration": 19.0, "agility": 19.0, "balance": 19.0, "jumping_reach": 7.0, "natural_fitness": 7.0, "pace": 15.0, "stamina": 17.0, "strength": 7.0}</t>
+          <t>{"darts": 16.0, "finishing": 9.0, "footwork": 8.0, "goal_kicking": 4.0, "handling": 7.0, "kicking": 6.0, "kicking_power": 3.0, "lineouts": 3.0, "marking": 9.0, "offloading": 18.0, "passing": 13.0, "scrummaging": 9.0, "rucking": 20.0, "technique": 20.0, "aggression": 6.0, "anticipation": 19.0, "bravery": 12.0, "composure": 4.0, "concentration": 7.0, "decisions": 15.0, "determination": 6.0, "flair": 7.0, "leadership": 13.0, "off_the_ball": 19.0, "positioning": 7.0, "teamwork": 20.0, "vision": 8.0, "work_rate": 14.0, "acceleration": 12.0, "agility": 5.0, "balance": 8.0, "jumping_reach": 5.0, "natural_fitness": 5.0, "pace": 7.0, "stamina": 20.0, "strength": 8.0}</t>
         </is>
       </c>
       <c r="AC4" t="inlineStr">
         <is>
-          <t>{"Consistency": 16.0, "Controversy": 7.3, "Dirtiness": 13.4, "Important Matches": 16.5, "Injury Proneness": 14.3, "Loyalty": 14.1, "Pressure": 16.7, "Professionalism": 16.9, "Sportsmanship": 3.3, "Temperament": 12.2, "Versatility": 12.7, "Ambition": 18.2, "Adaptability": 14.6}</t>
+          <t>{"Consistency": 14.3, "Controversy": 3.3, "Dirtiness": 3.9, "Important Matches": 15.8, "Injury Proneness": 9.6, "Loyalty": 16.3, "Pressure": 18.9, "Professionalism": 19.5, "Sportsmanship": 18.3, "Temperament": 17.4, "Versatility": 9.5, "Ambition": 18.2, "Adaptability": 19.7}</t>
         </is>
       </c>
     </row>
@@ -797,43 +791,41 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t xml:space="preserve">Andrew </t>
+          <t xml:space="preserve">Tadgh </t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Porter</t>
+          <t>Beirne</t>
         </is>
       </c>
       <c r="D5" s="2" t="n">
-        <v>34703</v>
+        <v>32877</v>
       </c>
       <c r="E5" t="n">
         <v>183</v>
       </c>
       <c r="F5" t="n">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="G5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H5" t="n">
-        <v>90</v>
-      </c>
-      <c r="I5" t="n">
-        <v>2</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr"/>
       <c r="M5" t="inlineStr"/>
       <c r="N5" t="inlineStr">
         <is>
-          <t>lp:5, tp:4</t>
+          <t>sr:5</t>
         </is>
       </c>
       <c r="O5" t="n">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="P5" t="inlineStr"/>
       <c r="Q5" t="inlineStr"/>
@@ -851,12 +843,12 @@
       <c r="AA5" t="inlineStr"/>
       <c r="AB5" t="inlineStr">
         <is>
-          <t>{"darts": 4.0, "finishing": 6.0, "footwork": 14.0, "goal_kicking": 3.0, "handling": 17.0, "kicking": 6.0, "kicking_power": 2.0, "lineouts": 2.0, "marking": 15.0, "offloading": 11.0, "passing": 9.0, "scrummaging": 19.0, "rucking": 15.0, "technique": 11.0, "aggression": 11.0, "anticipation": 20.0, "bravery": 15.0, "composure": 10.0, "concentration": 7.0, "decisions": 20.0, "determination": 18.0, "flair": 12.0, "leadership": 13.0, "off_the_ball": 12.0, "positioning": 11.0, "teamwork": 20.0, "vision": 2.0, "work_rate": 14.0, "acceleration": 11.0, "agility": 12.0, "balance": 18.0, "jumping_reach": 6.0, "natural_fitness": 15.0, "pace": 12.0, "stamina": 18.0, "strength": 20.0}</t>
+          <t>{"darts": 4.0, "finishing": 13.0, "footwork": 20.0, "goal_kicking": 5.0, "handling": 17.0, "kicking": 4.0, "kicking_power": 3.0, "lineouts": 7.0, "marking": 10.0, "offloading": 6.0, "passing": 18.0, "scrummaging": 8.0, "rucking": 6.0, "technique": 8.0, "aggression": 7.0, "anticipation": 6.0, "bravery": 18.0, "composure": 3.0, "concentration": 17.0, "decisions": 8.0, "determination": 17.0, "flair": 17.0, "leadership": 12.0, "off_the_ball": 10.0, "positioning": 13.0, "teamwork": 13.0, "vision": 16.0, "work_rate": 5.0, "acceleration": 16.0, "agility": 3.0, "balance": 7.0, "jumping_reach": 4.0, "natural_fitness": 18.0, "pace": 14.0, "stamina": 13.0, "strength": 6.0}</t>
         </is>
       </c>
       <c r="AC5" t="inlineStr">
         <is>
-          <t>{"Consistency": 16.7, "Controversy": 1.0, "Dirtiness": 3.5, "Important Matches": 17.2, "Injury Proneness": 12.6, "Loyalty": 16.7, "Pressure": 16.4, "Professionalism": 19.9, "Sportsmanship": 17.7, "Temperament": 19.4, "Versatility": 18.1, "Ambition": 19.7, "Adaptability": 19.1}</t>
+          <t>{"Consistency": 15.5, "Controversy": 3.9, "Dirtiness": 4.5, "Important Matches": 16.8, "Injury Proneness": 1.7, "Loyalty": 15.5, "Pressure": 15.5, "Professionalism": 19.6, "Sportsmanship": 18.5, "Temperament": 17.2, "Versatility": 5.0, "Ambition": 17.9, "Adaptability": 17.7}</t>
         </is>
       </c>
     </row>
@@ -866,43 +858,41 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rabbah </t>
+          <t xml:space="preserve">James </t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Slimani</t>
+          <t>Ryan</t>
         </is>
       </c>
       <c r="D6" s="2" t="n">
-        <v>32143</v>
+        <v>32878</v>
       </c>
       <c r="E6" t="n">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="F6" t="n">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="G6" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H6" t="n">
         <v>75</v>
       </c>
-      <c r="I6" t="n">
-        <v>2</v>
-      </c>
+      <c r="I6" t="inlineStr"/>
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr"/>
       <c r="M6" t="inlineStr"/>
       <c r="N6" t="inlineStr">
         <is>
-          <t>tp:5</t>
+          <t>sr:5</t>
         </is>
       </c>
       <c r="O6" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="P6" t="inlineStr"/>
       <c r="Q6" t="inlineStr"/>
@@ -920,12 +910,12 @@
       <c r="AA6" t="inlineStr"/>
       <c r="AB6" t="inlineStr">
         <is>
-          <t>{"darts": 3.0, "finishing": 5.0, "footwork": 14.0, "goal_kicking": 5.0, "handling": 16.0, "kicking": 7.0, "kicking_power": 4.0, "lineouts": 3.0, "marking": 14.0, "offloading": 10.0, "passing": 7.0, "scrummaging": 19.0, "rucking": 14.0, "technique": 3.0, "aggression": 14.0, "anticipation": 17.0, "bravery": 14.0, "composure": 8.0, "concentration": 8.0, "decisions": 9.0, "determination": 19.0, "flair": 6.0, "leadership": 20.0, "off_the_ball": 5.0, "positioning": 7.0, "teamwork": 16.0, "vision": 4.0, "work_rate": 14.0, "acceleration": 6.0, "agility": 7.0, "balance": 9.0, "jumping_reach": 5.0, "natural_fitness": 11.0, "pace": 5.0, "stamina": 7.0, "strength": 17.0}</t>
+          <t>{"darts": 3.0, "finishing": 11.0, "footwork": 3.0, "goal_kicking": 2.0, "handling": 17.0, "kicking": 4.0, "kicking_power": 3.0, "lineouts": 11.0, "marking": 18.0, "offloading": 5.0, "passing": 6.0, "scrummaging": 12.0, "rucking": 13.0, "technique": 7.0, "aggression": 9.0, "anticipation": 13.0, "bravery": 19.0, "composure": 2.0, "concentration": 4.0, "decisions": 17.0, "determination": 12.0, "flair": 10.0, "leadership": 6.0, "off_the_ball": 2.0, "positioning": 10.0, "teamwork": 12.0, "vision": 16.0, "work_rate": 11.0, "acceleration": 17.0, "agility": 11.0, "balance": 5.0, "jumping_reach": 9.0, "natural_fitness": 13.0, "pace": 10.0, "stamina": 8.0, "strength": 15.0}</t>
         </is>
       </c>
       <c r="AC6" t="inlineStr">
         <is>
-          <t>{"Consistency": 19.1, "Controversy": 3.9, "Dirtiness": 3.9, "Important Matches": 17.9, "Injury Proneness": 9.2, "Loyalty": 18.9, "Pressure": 16.1, "Professionalism": 18.6, "Sportsmanship": 17.4, "Temperament": 19.5, "Versatility": 1.2, "Ambition": 18.5, "Adaptability": 19.6}</t>
+          <t>{"Consistency": 18.7, "Controversy": 3.0, "Dirtiness": 3.0, "Important Matches": 17.6, "Injury Proneness": 11.7, "Loyalty": 14.1, "Pressure": 18.8, "Professionalism": 19.4, "Sportsmanship": 19.7, "Temperament": 18.8, "Versatility": 11.7, "Ambition": 17.0, "Adaptability": 19.7}</t>
         </is>
       </c>
     </row>
@@ -935,43 +925,41 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Ben</t>
+          <t>Ryan</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Tamueifena</t>
+          <t>Baird</t>
         </is>
       </c>
       <c r="D7" s="2" t="n">
-        <v>32144</v>
+        <v>32879</v>
       </c>
       <c r="E7" t="n">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="F7" t="n">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="G7" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="H7" t="n">
-        <v>80</v>
-      </c>
-      <c r="I7" t="n">
-        <v>16</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="I7" t="inlineStr"/>
       <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr"/>
       <c r="M7" t="inlineStr"/>
       <c r="N7" t="inlineStr">
         <is>
-          <t>tp:5</t>
+          <t>br:5</t>
         </is>
       </c>
       <c r="O7" t="n">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="P7" t="inlineStr"/>
       <c r="Q7" t="inlineStr"/>
@@ -982,19 +970,19 @@
       <c r="V7" t="inlineStr"/>
       <c r="W7" t="inlineStr"/>
       <c r="X7" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Y7" t="inlineStr"/>
       <c r="Z7" t="inlineStr"/>
       <c r="AA7" t="inlineStr"/>
       <c r="AB7" t="inlineStr">
         <is>
-          <t>{"darts": 2.0, "finishing": 9.0, "footwork": 16.0, "goal_kicking": 4.0, "handling": 16.0, "kicking": 1.0, "kicking_power": 4.0, "lineouts": 2.0, "marking": 20.0, "offloading": 19.0, "passing": 11.0, "scrummaging": 19.0, "rucking": 10.0, "technique": 13.0, "aggression": 8.0, "anticipation": 16.0, "bravery": 14.0, "composure": 9.0, "concentration": 12.0, "decisions": 15.0, "determination": 15.0, "flair": 17.0, "leadership": 9.0, "off_the_ball": 8.0, "positioning": 7.0, "teamwork": 14.0, "vision": 2.0, "work_rate": 16.0, "acceleration": 5.0, "agility": 7.0, "balance": 18.0, "jumping_reach": 4.0, "natural_fitness": 10.0, "pace": 2.0, "stamina": 8.0, "strength": 19.0}</t>
+          <t>{"darts": 7.0, "finishing": 6.0, "footwork": 15.0, "goal_kicking": 4.0, "handling": 7.0, "kicking": 4.0, "kicking_power": 6.0, "lineouts": 3.0, "marking": 9.0, "offloading": 9.0, "passing": 7.0, "scrummaging": 11.0, "rucking": 17.0, "technique": 6.0, "aggression": 7.0, "anticipation": 3.0, "bravery": 7.0, "composure": 20.0, "concentration": 7.0, "decisions": 15.0, "determination": 20.0, "flair": 11.0, "leadership": 3.0, "off_the_ball": 18.0, "positioning": 11.0, "teamwork": 8.0, "vision": 4.0, "work_rate": 15.0, "acceleration": 5.0, "agility": 16.0, "balance": 13.0, "jumping_reach": 19.0, "natural_fitness": 4.0, "pace": 17.0, "stamina": 20.0, "strength": 12.0}</t>
         </is>
       </c>
       <c r="AC7" t="inlineStr">
         <is>
-          <t>{"Consistency": 16.9, "Controversy": 4.7, "Dirtiness": 7.0, "Important Matches": 16.1, "Injury Proneness": 16.9, "Loyalty": 13.4, "Pressure": 17.4, "Professionalism": 15.1, "Sportsmanship": 13.6, "Temperament": 15.5, "Versatility": 7.4, "Ambition": 16.1, "Adaptability": 13.0}</t>
+          <t>{"Consistency": 19.1, "Controversy": 1.4, "Dirtiness": 3.0, "Important Matches": 19.2, "Injury Proneness": 3.3, "Loyalty": 19.7, "Pressure": 14.7, "Professionalism": 19.0, "Sportsmanship": 19.9, "Temperament": 17.8, "Versatility": 9.4, "Ambition": 19.6, "Adaptability": 17.3}</t>
         </is>
       </c>
     </row>
@@ -1004,43 +992,41 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Jack</t>
+          <t xml:space="preserve">Josh </t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Boyle</t>
+          <t xml:space="preserve">Van der Flier </t>
         </is>
       </c>
       <c r="D8" s="2" t="n">
-        <v>32145</v>
+        <v>32880</v>
       </c>
       <c r="E8" t="n">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F8" t="n">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="G8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H8" t="n">
-        <v>70</v>
-      </c>
-      <c r="I8" t="n">
-        <v>2</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="I8" t="inlineStr"/>
       <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr"/>
       <c r="M8" t="inlineStr"/>
       <c r="N8" t="inlineStr">
         <is>
-          <t>lp:5, tp:4</t>
+          <t>br:5</t>
         </is>
       </c>
       <c r="O8" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P8" t="inlineStr"/>
       <c r="Q8" t="inlineStr"/>
@@ -1051,19 +1037,19 @@
       <c r="V8" t="inlineStr"/>
       <c r="W8" t="inlineStr"/>
       <c r="X8" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="Y8" t="inlineStr"/>
       <c r="Z8" t="inlineStr"/>
       <c r="AA8" t="inlineStr"/>
       <c r="AB8" t="inlineStr">
         <is>
-          <t>{"darts": 5.0, "finishing": 9.0, "footwork": 19.0, "goal_kicking": 4.0, "handling": 13.0, "kicking": 4.0, "kicking_power": 6.0, "lineouts": 3.0, "marking": 17.0, "offloading": 18.0, "passing": 3.0, "scrummaging": 3.0, "rucking": 14.0, "technique": 6.0, "aggression": 12.0, "anticipation": 5.0, "bravery": 13.0, "composure": 8.0, "concentration": 13.0, "decisions": 12.0, "determination": 7.0, "flair": 13.0, "leadership": 14.0, "off_the_ball": 9.0, "positioning": 17.0, "teamwork": 2.0, "vision": 15.0, "work_rate": 6.0, "acceleration": 7.0, "agility": 13.0, "balance": 8.0, "jumping_reach": 10.0, "natural_fitness": 20.0, "pace": 14.0, "stamina": 6.0, "strength": 5.0}</t>
+          <t>{"darts": 8.0, "finishing": 17.0, "footwork": 13.0, "goal_kicking": 3.0, "handling": 2.0, "kicking": 8.0, "kicking_power": 5.0, "lineouts": 18.0, "marking": 14.0, "offloading": 13.0, "passing": 17.0, "scrummaging": 7.0, "rucking": 9.0, "technique": 4.0, "aggression": 11.0, "anticipation": 16.0, "bravery": 6.0, "composure": 10.0, "concentration": 5.0, "decisions": 12.0, "determination": 5.0, "flair": 14.0, "leadership": 3.0, "off_the_ball": 5.0, "positioning": 18.0, "teamwork": 15.0, "vision": 9.0, "work_rate": 10.0, "acceleration": 15.0, "agility": 15.0, "balance": 6.0, "jumping_reach": 7.0, "natural_fitness": 15.0, "pace": 12.0, "stamina": 13.0, "strength": 6.0}</t>
         </is>
       </c>
       <c r="AC8" t="inlineStr">
         <is>
-          <t>{"Consistency": 19.5, "Controversy": 4.1, "Dirtiness": 9.9, "Important Matches": 12.1, "Injury Proneness": 14.1, "Loyalty": 11.0, "Pressure": 11.4, "Professionalism": 11.0, "Sportsmanship": 9.4, "Temperament": 8.7, "Versatility": 8.5, "Ambition": 19.6, "Adaptability": 15.7}</t>
+          <t>{"Consistency": 17.0, "Controversy": 2.1, "Dirtiness": 3.1, "Important Matches": 18.8, "Injury Proneness": 18.3, "Loyalty": 16.7, "Pressure": 19.7, "Professionalism": 19.9, "Sportsmanship": 19.2, "Temperament": 19.2, "Versatility": 13.3, "Ambition": 19.7, "Adaptability": 19.9}</t>
         </is>
       </c>
     </row>
@@ -1073,43 +1059,41 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Jack</t>
+          <t xml:space="preserve">Jack </t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Aungier</t>
+          <t>Conan</t>
         </is>
       </c>
       <c r="D9" s="2" t="n">
-        <v>32146</v>
+        <v>32881</v>
       </c>
       <c r="E9" t="n">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F9" t="n">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="G9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H9" t="n">
-        <v>62</v>
-      </c>
-      <c r="I9" t="n">
-        <v>2</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="I9" t="inlineStr"/>
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr"/>
       <c r="L9" t="inlineStr"/>
       <c r="M9" t="inlineStr"/>
       <c r="N9" t="inlineStr">
         <is>
-          <t>tp:5</t>
+          <t>br:5</t>
         </is>
       </c>
       <c r="O9" t="n">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="P9" t="inlineStr"/>
       <c r="Q9" t="inlineStr"/>
@@ -1120,19 +1104,19 @@
       <c r="V9" t="inlineStr"/>
       <c r="W9" t="inlineStr"/>
       <c r="X9" t="n">
-        <v>28</v>
+        <v>1</v>
       </c>
       <c r="Y9" t="inlineStr"/>
       <c r="Z9" t="inlineStr"/>
       <c r="AA9" t="inlineStr"/>
       <c r="AB9" t="inlineStr">
         <is>
-          <t>{"darts": 5.0, "finishing": 4.0, "footwork": 5.0, "goal_kicking": 5.0, "handling": 5.0, "kicking": 2.0, "kicking_power": 6.0, "lineouts": 2.0, "marking": 7.0, "offloading": 6.0, "passing": 4.0, "scrummaging": 19.0, "rucking": 15.0, "technique": 3.0, "aggression": 10.0, "anticipation": 17.0, "bravery": 15.0, "composure": 8.0, "concentration": 7.0, "decisions": 6.0, "determination": 14.0, "flair": 5.0, "leadership": 18.0, "off_the_ball": 10.0, "positioning": 3.0, "teamwork": 12.0, "vision": 7.0, "work_rate": 13.0, "acceleration": 4.0, "agility": 2.0, "balance": 8.0, "jumping_reach": 3.0, "natural_fitness": 3.0, "pace": 7.0, "stamina": 10.0, "strength": 16.0}</t>
+          <t>{"darts": 7.0, "finishing": 9.0, "footwork": 13.0, "goal_kicking": 4.0, "handling": 19.0, "kicking": 6.0, "kicking_power": 9.0, "lineouts": 5.0, "marking": 7.0, "offloading": 15.0, "passing": 16.0, "scrummaging": 8.0, "rucking": 10.0, "technique": 12.0, "aggression": 3.0, "anticipation": 2.0, "bravery": 18.0, "composure": 8.0, "concentration": 14.0, "decisions": 19.0, "determination": 5.0, "flair": 3.0, "leadership": 5.0, "off_the_ball": 16.0, "positioning": 18.0, "teamwork": 8.0, "vision": 18.0, "work_rate": 7.0, "acceleration": 4.0, "agility": 16.0, "balance": 19.0, "jumping_reach": 5.0, "natural_fitness": 9.0, "pace": 15.0, "stamina": 3.0, "strength": 14.0}</t>
         </is>
       </c>
       <c r="AC9" t="inlineStr">
         <is>
-          <t>{"Consistency": 8.7, "Controversy": 9.3, "Dirtiness": 11.8, "Important Matches": 9.7, "Injury Proneness": 4.7, "Loyalty": 9.5, "Pressure": 6.3, "Professionalism": 14.6, "Sportsmanship": 6.2, "Temperament": 11.1, "Versatility": 2.1, "Ambition": 11.4, "Adaptability": 8.7}</t>
+          <t>{"Consistency": 17.9, "Controversy": 3.7, "Dirtiness": 4.6, "Important Matches": 16.9, "Injury Proneness": 1.0, "Loyalty": 19.4, "Pressure": 17.8, "Professionalism": 18.8, "Sportsmanship": 17.7, "Temperament": 20.0, "Versatility": 19.3, "Ambition": 17.7, "Adaptability": 19.6}</t>
         </is>
       </c>
     </row>
@@ -1142,43 +1126,41 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Test</t>
+          <t>Jamison</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Clubman</t>
+          <t>Gibson-Park</t>
         </is>
       </c>
       <c r="D10" s="2" t="n">
-        <v>32147</v>
+        <v>32882</v>
       </c>
       <c r="E10" t="n">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F10" t="n">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="G10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H10" t="n">
-        <v>45</v>
-      </c>
-      <c r="I10" t="n">
-        <v>2</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="I10" t="inlineStr"/>
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr"/>
       <c r="L10" t="inlineStr"/>
       <c r="M10" t="inlineStr"/>
       <c r="N10" t="inlineStr">
         <is>
-          <t>tp:5</t>
+          <t>sh:5</t>
         </is>
       </c>
       <c r="O10" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="P10" t="inlineStr"/>
       <c r="Q10" t="inlineStr"/>
@@ -1189,19 +1171,2498 @@
       <c r="V10" t="inlineStr"/>
       <c r="W10" t="inlineStr"/>
       <c r="X10" t="n">
-        <v>28</v>
+        <v>1</v>
       </c>
       <c r="Y10" t="inlineStr"/>
       <c r="Z10" t="inlineStr"/>
       <c r="AA10" t="inlineStr"/>
       <c r="AB10" t="inlineStr">
         <is>
-          <t>{"darts": 7.0, "finishing": 8.0, "footwork": 7.0, "goal_kicking": 2.0, "handling": 12.0, "kicking": 2.0, "kicking_power": 2.0, "lineouts": 1.0, "marking": 9.0, "offloading": 2.0, "passing": 10.0, "scrummaging": 14.0, "rucking": 2.0, "technique": 2.0, "aggression": 1.0, "anticipation": 6.0, "bravery": 10.0, "composure": 13.0, "concentration": 11.0, "decisions": 2.0, "determination": 10.0, "flair": 2.0, "leadership": 5.0, "off_the_ball": 10.0, "positioning": 7.0, "teamwork": 15.0, "vision": 16.0, "work_rate": 1.0, "acceleration": 1.0, "agility": 1.0, "balance": 3.0, "jumping_reach": 4.0, "natural_fitness": 5.0, "pace": 3.0, "stamina": 13.0, "strength": 5.0}</t>
+          <t>{"darts": 3.0, "finishing": 14.0, "footwork": 4.0, "goal_kicking": 20.0, "handling": 3.0, "kicking": 12.0, "kicking_power": 20.0, "lineouts": 6.0, "marking": 3.0, "offloading": 16.0, "passing": 17.0, "scrummaging": 17.0, "rucking": 6.0, "technique": 4.0, "aggression": 3.0, "anticipation": 11.0, "bravery": 7.0, "composure": 16.0, "concentration": 18.0, "decisions": 10.0, "determination": 8.0, "flair": 16.0, "leadership": 8.0, "off_the_ball": 5.0, "positioning": 8.0, "teamwork": 18.0, "vision": 5.0, "work_rate": 12.0, "acceleration": 4.0, "agility": 19.0, "balance": 8.0, "jumping_reach": 9.0, "natural_fitness": 8.0, "pace": 11.0, "stamina": 5.0, "strength": 17.0}</t>
         </is>
       </c>
       <c r="AC10" t="inlineStr">
         <is>
-          <t>{"Consistency": 9.7, "Controversy": 8.4, "Dirtiness": 11.2, "Important Matches": 8.2, "Injury Proneness": 11.3, "Loyalty": 8.8, "Pressure": 7.6, "Professionalism": 8.5, "Sportsmanship": 5.5, "Temperament": 9.2, "Versatility": 14.5, "Ambition": 9.7, "Adaptability": 8.4}</t>
+          <t>{"Consistency": 18.7, "Controversy": 4.6, "Dirtiness": 3.5, "Important Matches": 14.8, "Injury Proneness": 7.7, "Loyalty": 14.2, "Pressure": 18.7, "Professionalism": 19.3, "Sportsmanship": 18.1, "Temperament": 18.0, "Versatility": 14.6, "Ambition": 17.0, "Adaptability": 18.8}</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Jack </t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Crowley</t>
+        </is>
+      </c>
+      <c r="D11" s="2" t="n">
+        <v>32883</v>
+      </c>
+      <c r="E11" t="n">
+        <v>183</v>
+      </c>
+      <c r="F11" t="n">
+        <v>100</v>
+      </c>
+      <c r="G11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H11" t="n">
+        <v>75</v>
+      </c>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr"/>
+      <c r="M11" t="inlineStr"/>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>fh:5</t>
+        </is>
+      </c>
+      <c r="O11" t="n">
+        <v>7</v>
+      </c>
+      <c r="P11" t="inlineStr"/>
+      <c r="Q11" t="inlineStr"/>
+      <c r="R11" t="inlineStr"/>
+      <c r="S11" t="inlineStr"/>
+      <c r="T11" t="inlineStr"/>
+      <c r="U11" t="inlineStr"/>
+      <c r="V11" t="inlineStr"/>
+      <c r="W11" t="inlineStr"/>
+      <c r="X11" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y11" t="inlineStr"/>
+      <c r="Z11" t="inlineStr"/>
+      <c r="AA11" t="inlineStr"/>
+      <c r="AB11" t="inlineStr">
+        <is>
+          <t>{"darts": 4.0, "finishing": 7.0, "footwork": 5.0, "goal_kicking": 16.0, "handling": 19.0, "kicking": 16.0, "kicking_power": 20.0, "lineouts": 10.0, "marking": 17.0, "offloading": 15.0, "passing": 11.0, "scrummaging": 3.0, "rucking": 19.0, "technique": 8.0, "aggression": 19.0, "anticipation": 6.0, "bravery": 17.0, "composure": 19.0, "concentration": 10.0, "decisions": 19.0, "determination": 2.0, "flair": 8.0, "leadership": 10.0, "off_the_ball": 12.0, "positioning": 8.0, "teamwork": 3.0, "vision": 14.0, "work_rate": 5.0, "acceleration": 9.0, "agility": 11.0, "balance": 3.0, "jumping_reach": 4.0, "natural_fitness": 4.0, "pace": 13.0, "stamina": 7.0, "strength": 3.0}</t>
+        </is>
+      </c>
+      <c r="AC11" t="inlineStr">
+        <is>
+          <t>{"Consistency": 14.6, "Controversy": 1.5, "Dirtiness": 3.5, "Important Matches": 15.4, "Injury Proneness": 5.4, "Loyalty": 15.0, "Pressure": 14.6, "Professionalism": 19.7, "Sportsmanship": 18.4, "Temperament": 17.9, "Versatility": 7.0, "Ambition": 17.2, "Adaptability": 18.2}</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">James </t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Lowe</t>
+        </is>
+      </c>
+      <c r="D12" s="2" t="n">
+        <v>32884</v>
+      </c>
+      <c r="E12" t="n">
+        <v>183</v>
+      </c>
+      <c r="F12" t="n">
+        <v>100</v>
+      </c>
+      <c r="G12" t="n">
+        <v>1</v>
+      </c>
+      <c r="H12" t="n">
+        <v>75</v>
+      </c>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="inlineStr"/>
+      <c r="M12" t="inlineStr"/>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>wg:5</t>
+        </is>
+      </c>
+      <c r="O12" t="n">
+        <v>9</v>
+      </c>
+      <c r="P12" t="inlineStr"/>
+      <c r="Q12" t="inlineStr"/>
+      <c r="R12" t="inlineStr"/>
+      <c r="S12" t="inlineStr"/>
+      <c r="T12" t="inlineStr"/>
+      <c r="U12" t="inlineStr"/>
+      <c r="V12" t="inlineStr"/>
+      <c r="W12" t="inlineStr"/>
+      <c r="X12" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y12" t="inlineStr"/>
+      <c r="Z12" t="inlineStr"/>
+      <c r="AA12" t="inlineStr"/>
+      <c r="AB12" t="inlineStr">
+        <is>
+          <t>{"darts": 2.0, "finishing": 11.0, "footwork": 4.0, "goal_kicking": 13.0, "handling": 6.0, "kicking": 4.0, "kicking_power": 13.0, "lineouts": 2.0, "marking": 17.0, "offloading": 14.0, "passing": 19.0, "scrummaging": 13.0, "rucking": 10.0, "technique": 9.0, "aggression": 9.0, "anticipation": 14.0, "bravery": 8.0, "composure": 11.0, "concentration": 19.0, "decisions": 3.0, "determination": 20.0, "flair": 15.0, "leadership": 2.0, "off_the_ball": 2.0, "positioning": 11.0, "teamwork": 19.0, "vision": 3.0, "work_rate": 10.0, "acceleration": 3.0, "agility": 13.0, "balance": 15.0, "jumping_reach": 7.0, "natural_fitness": 19.0, "pace": 6.0, "stamina": 4.0, "strength": 16.0}</t>
+        </is>
+      </c>
+      <c r="AC12" t="inlineStr">
+        <is>
+          <t>{"Consistency": 17.2, "Controversy": 4.7, "Dirtiness": 3.5, "Important Matches": 15.8, "Injury Proneness": 13.2, "Loyalty": 14.5, "Pressure": 16.4, "Professionalism": 18.6, "Sportsmanship": 19.0, "Temperament": 19.2, "Versatility": 7.6, "Ambition": 17.7, "Adaptability": 19.8}</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Bundee</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Aki</t>
+        </is>
+      </c>
+      <c r="D13" s="2" t="n">
+        <v>32885</v>
+      </c>
+      <c r="E13" t="n">
+        <v>183</v>
+      </c>
+      <c r="F13" t="n">
+        <v>100</v>
+      </c>
+      <c r="G13" t="n">
+        <v>1</v>
+      </c>
+      <c r="H13" t="n">
+        <v>75</v>
+      </c>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr"/>
+      <c r="M13" t="inlineStr"/>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>ct:5</t>
+        </is>
+      </c>
+      <c r="O13" t="n">
+        <v>8</v>
+      </c>
+      <c r="P13" t="inlineStr"/>
+      <c r="Q13" t="inlineStr"/>
+      <c r="R13" t="inlineStr"/>
+      <c r="S13" t="inlineStr"/>
+      <c r="T13" t="inlineStr"/>
+      <c r="U13" t="inlineStr"/>
+      <c r="V13" t="inlineStr"/>
+      <c r="W13" t="inlineStr"/>
+      <c r="X13" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y13" t="inlineStr"/>
+      <c r="Z13" t="inlineStr"/>
+      <c r="AA13" t="inlineStr"/>
+      <c r="AB13" t="inlineStr">
+        <is>
+          <t>{"darts": 5.0, "finishing": 5.0, "footwork": 18.0, "goal_kicking": 11.0, "handling": 11.0, "kicking": 6.0, "kicking_power": 16.0, "lineouts": 5.0, "marking": 15.0, "offloading": 14.0, "passing": 12.0, "scrummaging": 14.0, "rucking": 11.0, "technique": 17.0, "aggression": 1.0, "anticipation": 20.0, "bravery": 18.0, "composure": 5.0, "concentration": 13.0, "decisions": 1.0, "determination": 9.0, "flair": 15.0, "leadership": 6.0, "off_the_ball": 16.0, "positioning": 3.0, "teamwork": 6.0, "vision": 15.0, "work_rate": 9.0, "acceleration": 19.0, "agility": 9.0, "balance": 1.0, "jumping_reach": 13.0, "natural_fitness": 8.0, "pace": 14.0, "stamina": 9.0, "strength": 2.0}</t>
+        </is>
+      </c>
+      <c r="AC13" t="inlineStr">
+        <is>
+          <t>{"Consistency": 15.9, "Controversy": 1.2, "Dirtiness": 2.4, "Important Matches": 17.7, "Injury Proneness": 8.9, "Loyalty": 17.6, "Pressure": 17.6, "Professionalism": 19.3, "Sportsmanship": 17.6, "Temperament": 19.0, "Versatility": 16.3, "Ambition": 17.6, "Adaptability": 17.9}</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gary </t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Ringrose</t>
+        </is>
+      </c>
+      <c r="D14" s="2" t="n">
+        <v>32886</v>
+      </c>
+      <c r="E14" t="n">
+        <v>183</v>
+      </c>
+      <c r="F14" t="n">
+        <v>100</v>
+      </c>
+      <c r="G14" t="n">
+        <v>1</v>
+      </c>
+      <c r="H14" t="n">
+        <v>75</v>
+      </c>
+      <c r="I14" t="inlineStr"/>
+      <c r="J14" t="inlineStr"/>
+      <c r="K14" t="inlineStr"/>
+      <c r="L14" t="inlineStr"/>
+      <c r="M14" t="inlineStr"/>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>ct:5</t>
+        </is>
+      </c>
+      <c r="O14" t="n">
+        <v>8</v>
+      </c>
+      <c r="P14" t="inlineStr"/>
+      <c r="Q14" t="inlineStr"/>
+      <c r="R14" t="inlineStr"/>
+      <c r="S14" t="inlineStr"/>
+      <c r="T14" t="inlineStr"/>
+      <c r="U14" t="inlineStr"/>
+      <c r="V14" t="inlineStr"/>
+      <c r="W14" t="inlineStr"/>
+      <c r="X14" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y14" t="inlineStr"/>
+      <c r="Z14" t="inlineStr"/>
+      <c r="AA14" t="inlineStr"/>
+      <c r="AB14" t="inlineStr">
+        <is>
+          <t>{"darts": 2.0, "finishing": 12.0, "footwork": 9.0, "goal_kicking": 16.0, "handling": 5.0, "kicking": 8.0, "kicking_power": 16.0, "lineouts": 6.0, "marking": 15.0, "offloading": 11.0, "passing": 15.0, "scrummaging": 7.0, "rucking": 16.0, "technique": 13.0, "aggression": 9.0, "anticipation": 7.0, "bravery": 6.0, "composure": 17.0, "concentration": 11.0, "decisions": 14.0, "determination": 5.0, "flair": 4.0, "leadership": 12.0, "off_the_ball": 11.0, "positioning": 6.0, "teamwork": 19.0, "vision": 19.0, "work_rate": 8.0, "acceleration": 6.0, "agility": 19.0, "balance": 8.0, "jumping_reach": 10.0, "natural_fitness": 11.0, "pace": 4.0, "stamina": 19.0, "strength": 7.0}</t>
+        </is>
+      </c>
+      <c r="AC14" t="inlineStr">
+        <is>
+          <t>{"Consistency": 17.2, "Controversy": 3.7, "Dirtiness": 3.6, "Important Matches": 19.3, "Injury Proneness": 7.5, "Loyalty": 15.3, "Pressure": 15.1, "Professionalism": 19.5, "Sportsmanship": 18.7, "Temperament": 18.4, "Versatility": 16.7, "Ambition": 19.4, "Adaptability": 18.9}</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Mack</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Hansen</t>
+        </is>
+      </c>
+      <c r="D15" s="2" t="n">
+        <v>32887</v>
+      </c>
+      <c r="E15" t="n">
+        <v>183</v>
+      </c>
+      <c r="F15" t="n">
+        <v>100</v>
+      </c>
+      <c r="G15" t="n">
+        <v>1</v>
+      </c>
+      <c r="H15" t="n">
+        <v>75</v>
+      </c>
+      <c r="I15" t="inlineStr"/>
+      <c r="J15" t="inlineStr"/>
+      <c r="K15" t="inlineStr"/>
+      <c r="L15" t="inlineStr"/>
+      <c r="M15" t="inlineStr"/>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>wg:5</t>
+        </is>
+      </c>
+      <c r="O15" t="n">
+        <v>9</v>
+      </c>
+      <c r="P15" t="inlineStr"/>
+      <c r="Q15" t="inlineStr"/>
+      <c r="R15" t="inlineStr"/>
+      <c r="S15" t="inlineStr"/>
+      <c r="T15" t="inlineStr"/>
+      <c r="U15" t="inlineStr"/>
+      <c r="V15" t="inlineStr"/>
+      <c r="W15" t="inlineStr"/>
+      <c r="X15" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y15" t="inlineStr"/>
+      <c r="Z15" t="inlineStr"/>
+      <c r="AA15" t="inlineStr"/>
+      <c r="AB15" t="inlineStr">
+        <is>
+          <t>{"darts": 3.0, "finishing": 8.0, "footwork": 13.0, "goal_kicking": 6.0, "handling": 13.0, "kicking": 19.0, "kicking_power": 20.0, "lineouts": 4.0, "marking": 15.0, "offloading": 6.0, "passing": 15.0, "scrummaging": 10.0, "rucking": 16.0, "technique": 4.0, "aggression": 10.0, "anticipation": 1.0, "bravery": 3.0, "composure": 6.0, "concentration": 18.0, "decisions": 19.0, "determination": 5.0, "flair": 9.0, "leadership": 18.0, "off_the_ball": 19.0, "positioning": 14.0, "teamwork": 16.0, "vision": 18.0, "work_rate": 3.0, "acceleration": 15.0, "agility": 3.0, "balance": 20.0, "jumping_reach": 6.0, "natural_fitness": 9.0, "pace": 4.0, "stamina": 9.0, "strength": 8.0}</t>
+        </is>
+      </c>
+      <c r="AC15" t="inlineStr">
+        <is>
+          <t>{"Consistency": 18.3, "Controversy": 1.4, "Dirtiness": 2.4, "Important Matches": 14.1, "Injury Proneness": 5.6, "Loyalty": 16.5, "Pressure": 14.5, "Professionalism": 19.3, "Sportsmanship": 18.6, "Temperament": 17.6, "Versatility": 7.6, "Ambition": 19.5, "Adaptability": 17.5}</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Hugo</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Keenan</t>
+        </is>
+      </c>
+      <c r="D16" s="2" t="n">
+        <v>32888</v>
+      </c>
+      <c r="E16" t="n">
+        <v>183</v>
+      </c>
+      <c r="F16" t="n">
+        <v>100</v>
+      </c>
+      <c r="G16" t="n">
+        <v>1</v>
+      </c>
+      <c r="H16" t="n">
+        <v>75</v>
+      </c>
+      <c r="I16" t="inlineStr"/>
+      <c r="J16" t="inlineStr"/>
+      <c r="K16" t="inlineStr"/>
+      <c r="L16" t="inlineStr"/>
+      <c r="M16" t="inlineStr"/>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>fb:5</t>
+        </is>
+      </c>
+      <c r="O16" t="n">
+        <v>10</v>
+      </c>
+      <c r="P16" t="inlineStr"/>
+      <c r="Q16" t="inlineStr"/>
+      <c r="R16" t="inlineStr"/>
+      <c r="S16" t="inlineStr"/>
+      <c r="T16" t="inlineStr"/>
+      <c r="U16" t="inlineStr"/>
+      <c r="V16" t="inlineStr"/>
+      <c r="W16" t="inlineStr"/>
+      <c r="X16" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y16" t="inlineStr"/>
+      <c r="Z16" t="inlineStr"/>
+      <c r="AA16" t="inlineStr"/>
+      <c r="AB16" t="inlineStr">
+        <is>
+          <t>{"darts": 3.0, "finishing": 9.0, "footwork": 14.0, "goal_kicking": 15.0, "handling": 13.0, "kicking": 9.0, "kicking_power": 17.0, "lineouts": 9.0, "marking": 1.0, "offloading": 7.0, "passing": 16.0, "scrummaging": 10.0, "rucking": 2.0, "technique": 4.0, "aggression": 13.0, "anticipation": 2.0, "bravery": 17.0, "composure": 6.0, "concentration": 18.0, "decisions": 12.0, "determination": 16.0, "flair": 17.0, "leadership": 1.0, "off_the_ball": 18.0, "positioning": 12.0, "teamwork": 7.0, "vision": 12.0, "work_rate": 14.0, "acceleration": 16.0, "agility": 10.0, "balance": 10.0, "jumping_reach": 10.0, "natural_fitness": 4.0, "pace": 12.0, "stamina": 3.0, "strength": 9.0}</t>
+        </is>
+      </c>
+      <c r="AC16" t="inlineStr">
+        <is>
+          <t>{"Consistency": 14.5, "Controversy": 2.3, "Dirtiness": 1.4, "Important Matches": 14.3, "Injury Proneness": 17.6, "Loyalty": 14.4, "Pressure": 15.0, "Professionalism": 19.9, "Sportsmanship": 17.4, "Temperament": 17.7, "Versatility": 18.7, "Ambition": 19.4, "Adaptability": 17.9}</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Ronan</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Kelleher</t>
+        </is>
+      </c>
+      <c r="D17" s="2" t="n">
+        <v>32889</v>
+      </c>
+      <c r="E17" t="n">
+        <v>183</v>
+      </c>
+      <c r="F17" t="n">
+        <v>100</v>
+      </c>
+      <c r="G17" t="n">
+        <v>1</v>
+      </c>
+      <c r="H17" t="n">
+        <v>75</v>
+      </c>
+      <c r="I17" t="inlineStr"/>
+      <c r="J17" t="inlineStr"/>
+      <c r="K17" t="inlineStr"/>
+      <c r="L17" t="inlineStr"/>
+      <c r="M17" t="inlineStr"/>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>hk:5</t>
+        </is>
+      </c>
+      <c r="O17" t="n">
+        <v>3</v>
+      </c>
+      <c r="P17" t="inlineStr"/>
+      <c r="Q17" t="inlineStr"/>
+      <c r="R17" t="inlineStr"/>
+      <c r="S17" t="inlineStr"/>
+      <c r="T17" t="inlineStr"/>
+      <c r="U17" t="inlineStr"/>
+      <c r="V17" t="inlineStr"/>
+      <c r="W17" t="inlineStr"/>
+      <c r="X17" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y17" t="inlineStr"/>
+      <c r="Z17" t="inlineStr"/>
+      <c r="AA17" t="inlineStr"/>
+      <c r="AB17" t="inlineStr">
+        <is>
+          <t>{"darts": 15.0, "finishing": 6.0, "footwork": 9.0, "goal_kicking": 5.0, "handling": 4.0, "kicking": 8.0, "kicking_power": 9.0, "lineouts": 7.0, "marking": 19.0, "offloading": 20.0, "passing": 11.0, "scrummaging": 15.0, "rucking": 3.0, "technique": 18.0, "aggression": 8.0, "anticipation": 6.0, "bravery": 12.0, "composure": 4.0, "concentration": 17.0, "decisions": 7.0, "determination": 16.0, "flair": 9.0, "leadership": 14.0, "off_the_ball": 11.0, "positioning": 19.0, "teamwork": 10.0, "vision": 3.0, "work_rate": 8.0, "acceleration": 14.0, "agility": 3.0, "balance": 8.0, "jumping_reach": 6.0, "natural_fitness": 8.0, "pace": 2.0, "stamina": 18.0, "strength": 8.0}</t>
+        </is>
+      </c>
+      <c r="AC17" t="inlineStr">
+        <is>
+          <t>{"Consistency": 18.1, "Controversy": 3.1, "Dirtiness": 2.2, "Important Matches": 16.9, "Injury Proneness": 1.9, "Loyalty": 14.7, "Pressure": 18.1, "Professionalism": 18.2, "Sportsmanship": 18.6, "Temperament": 19.1, "Versatility": 13.2, "Ambition": 18.0, "Adaptability": 19.5}</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Cian</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Healy</t>
+        </is>
+      </c>
+      <c r="D18" s="2" t="n">
+        <v>32890</v>
+      </c>
+      <c r="E18" t="n">
+        <v>183</v>
+      </c>
+      <c r="F18" t="n">
+        <v>100</v>
+      </c>
+      <c r="G18" t="n">
+        <v>1</v>
+      </c>
+      <c r="H18" t="n">
+        <v>75</v>
+      </c>
+      <c r="I18" t="inlineStr"/>
+      <c r="J18" t="inlineStr"/>
+      <c r="K18" t="inlineStr"/>
+      <c r="L18" t="inlineStr"/>
+      <c r="M18" t="inlineStr"/>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>lp:5</t>
+        </is>
+      </c>
+      <c r="O18" t="n">
+        <v>1</v>
+      </c>
+      <c r="P18" t="inlineStr"/>
+      <c r="Q18" t="inlineStr"/>
+      <c r="R18" t="inlineStr"/>
+      <c r="S18" t="inlineStr"/>
+      <c r="T18" t="inlineStr"/>
+      <c r="U18" t="inlineStr"/>
+      <c r="V18" t="inlineStr"/>
+      <c r="W18" t="inlineStr"/>
+      <c r="X18" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y18" t="inlineStr"/>
+      <c r="Z18" t="inlineStr"/>
+      <c r="AA18" t="inlineStr"/>
+      <c r="AB18" t="inlineStr">
+        <is>
+          <t>{"darts": 4.0, "finishing": 6.0, "footwork": 6.0, "goal_kicking": 4.0, "handling": 2.0, "kicking": 7.0, "kicking_power": 5.0, "lineouts": 2.0, "marking": 7.0, "offloading": 17.0, "passing": 17.0, "scrummaging": 17.0, "rucking": 16.0, "technique": 4.0, "aggression": 15.0, "anticipation": 19.0, "bravery": 5.0, "composure": 11.0, "concentration": 15.0, "decisions": 14.0, "determination": 19.0, "flair": 14.0, "leadership": 6.0, "off_the_ball": 8.0, "positioning": 12.0, "teamwork": 13.0, "vision": 6.0, "work_rate": 7.0, "acceleration": 9.0, "agility": 10.0, "balance": 17.0, "jumping_reach": 5.0, "natural_fitness": 5.0, "pace": 13.0, "stamina": 5.0, "strength": 19.0}</t>
+        </is>
+      </c>
+      <c r="AC18" t="inlineStr">
+        <is>
+          <t>{"Consistency": 17.3, "Controversy": 1.5, "Dirtiness": 4.2, "Important Matches": 17.1, "Injury Proneness": 6.6, "Loyalty": 17.8, "Pressure": 15.7, "Professionalism": 19.4, "Sportsmanship": 17.4, "Temperament": 17.9, "Versatility": 14.3, "Ambition": 18.9, "Adaptability": 17.4}</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Finlay</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Bealham</t>
+        </is>
+      </c>
+      <c r="D19" s="2" t="n">
+        <v>32891</v>
+      </c>
+      <c r="E19" t="n">
+        <v>183</v>
+      </c>
+      <c r="F19" t="n">
+        <v>100</v>
+      </c>
+      <c r="G19" t="n">
+        <v>1</v>
+      </c>
+      <c r="H19" t="n">
+        <v>75</v>
+      </c>
+      <c r="I19" t="inlineStr"/>
+      <c r="J19" t="inlineStr"/>
+      <c r="K19" t="inlineStr"/>
+      <c r="L19" t="inlineStr"/>
+      <c r="M19" t="inlineStr"/>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>tp:5</t>
+        </is>
+      </c>
+      <c r="O19" t="n">
+        <v>2</v>
+      </c>
+      <c r="P19" t="inlineStr"/>
+      <c r="Q19" t="inlineStr"/>
+      <c r="R19" t="inlineStr"/>
+      <c r="S19" t="inlineStr"/>
+      <c r="T19" t="inlineStr"/>
+      <c r="U19" t="inlineStr"/>
+      <c r="V19" t="inlineStr"/>
+      <c r="W19" t="inlineStr"/>
+      <c r="X19" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y19" t="inlineStr"/>
+      <c r="Z19" t="inlineStr"/>
+      <c r="AA19" t="inlineStr"/>
+      <c r="AB19" t="inlineStr">
+        <is>
+          <t>{"darts": 20.0, "finishing": 11.0, "footwork": 16.0, "goal_kicking": 2.0, "handling": 4.0, "kicking": 4.0, "kicking_power": 4.0, "lineouts": 3.0, "marking": 8.0, "offloading": 13.0, "passing": 11.0, "scrummaging": 17.0, "rucking": 7.0, "technique": 15.0, "aggression": 17.0, "anticipation": 20.0, "bravery": 5.0, "composure": 5.0, "concentration": 9.0, "decisions": 4.0, "determination": 8.0, "flair": 18.0, "leadership": 4.0, "off_the_ball": 6.0, "positioning": 8.0, "teamwork": 11.0, "vision": 11.0, "work_rate": 17.0, "acceleration": 2.0, "agility": 9.0, "balance": 15.0, "jumping_reach": 3.0, "natural_fitness": 8.0, "pace": 9.0, "stamina": 9.0, "strength": 18.0}</t>
+        </is>
+      </c>
+      <c r="AC19" t="inlineStr">
+        <is>
+          <t>{"Consistency": 19.1, "Controversy": 4.2, "Dirtiness": 1.0, "Important Matches": 14.2, "Injury Proneness": 9.8, "Loyalty": 19.3, "Pressure": 19.1, "Professionalism": 18.5, "Sportsmanship": 19.2, "Temperament": 18.3, "Versatility": 5.1, "Ambition": 18.0, "Adaptability": 19.3}</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Iain </t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Henderson</t>
+        </is>
+      </c>
+      <c r="D20" s="2" t="n">
+        <v>32892</v>
+      </c>
+      <c r="E20" t="n">
+        <v>183</v>
+      </c>
+      <c r="F20" t="n">
+        <v>100</v>
+      </c>
+      <c r="G20" t="n">
+        <v>1</v>
+      </c>
+      <c r="H20" t="n">
+        <v>75</v>
+      </c>
+      <c r="I20" t="inlineStr"/>
+      <c r="J20" t="inlineStr"/>
+      <c r="K20" t="inlineStr"/>
+      <c r="L20" t="inlineStr"/>
+      <c r="M20" t="inlineStr"/>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>sr:5</t>
+        </is>
+      </c>
+      <c r="O20" t="n">
+        <v>4</v>
+      </c>
+      <c r="P20" t="inlineStr"/>
+      <c r="Q20" t="inlineStr"/>
+      <c r="R20" t="inlineStr"/>
+      <c r="S20" t="inlineStr"/>
+      <c r="T20" t="inlineStr"/>
+      <c r="U20" t="inlineStr"/>
+      <c r="V20" t="inlineStr"/>
+      <c r="W20" t="inlineStr"/>
+      <c r="X20" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y20" t="inlineStr"/>
+      <c r="Z20" t="inlineStr"/>
+      <c r="AA20" t="inlineStr"/>
+      <c r="AB20" t="inlineStr">
+        <is>
+          <t>{"darts": 4.0, "finishing": 6.0, "footwork": 12.0, "goal_kicking": 3.0, "handling": 19.0, "kicking": 1.0, "kicking_power": 5.0, "lineouts": 20.0, "marking": 15.0, "offloading": 16.0, "passing": 9.0, "scrummaging": 12.0, "rucking": 14.0, "technique": 5.0, "aggression": 9.0, "anticipation": 13.0, "bravery": 4.0, "composure": 12.0, "concentration": 15.0, "decisions": 6.0, "determination": 19.0, "flair": 18.0, "leadership": 6.0, "off_the_ball": 5.0, "positioning": 3.0, "teamwork": 7.0, "vision": 8.0, "work_rate": 7.0, "acceleration": 13.0, "agility": 16.0, "balance": 5.0, "jumping_reach": 7.0, "natural_fitness": 9.0, "pace": 19.0, "stamina": 6.0, "strength": 7.0}</t>
+        </is>
+      </c>
+      <c r="AC20" t="inlineStr">
+        <is>
+          <t>{"Consistency": 15.6, "Controversy": 3.1, "Dirtiness": 2.5, "Important Matches": 14.4, "Injury Proneness": 14.7, "Loyalty": 16.4, "Pressure": 16.7, "Professionalism": 18.1, "Sportsmanship": 17.5, "Temperament": 19.6, "Versatility": 13.6, "Ambition": 19.7, "Adaptability": 19.2}</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Jack </t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Conan</t>
+        </is>
+      </c>
+      <c r="D21" s="2" t="n">
+        <v>32893</v>
+      </c>
+      <c r="E21" t="n">
+        <v>183</v>
+      </c>
+      <c r="F21" t="n">
+        <v>100</v>
+      </c>
+      <c r="G21" t="n">
+        <v>1</v>
+      </c>
+      <c r="H21" t="n">
+        <v>75</v>
+      </c>
+      <c r="I21" t="inlineStr"/>
+      <c r="J21" t="inlineStr"/>
+      <c r="K21" t="inlineStr"/>
+      <c r="L21" t="inlineStr"/>
+      <c r="M21" t="inlineStr"/>
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>br:5</t>
+        </is>
+      </c>
+      <c r="O21" t="n">
+        <v>5</v>
+      </c>
+      <c r="P21" t="inlineStr"/>
+      <c r="Q21" t="inlineStr"/>
+      <c r="R21" t="inlineStr"/>
+      <c r="S21" t="inlineStr"/>
+      <c r="T21" t="inlineStr"/>
+      <c r="U21" t="inlineStr"/>
+      <c r="V21" t="inlineStr"/>
+      <c r="W21" t="inlineStr"/>
+      <c r="X21" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y21" t="inlineStr"/>
+      <c r="Z21" t="inlineStr"/>
+      <c r="AA21" t="inlineStr"/>
+      <c r="AB21" t="inlineStr">
+        <is>
+          <t>{"darts": 11.0, "finishing": 12.0, "footwork": 2.0, "goal_kicking": 2.0, "handling": 13.0, "kicking": 3.0, "kicking_power": 3.0, "lineouts": 4.0, "marking": 19.0, "offloading": 15.0, "passing": 19.0, "scrummaging": 10.0, "rucking": 6.0, "technique": 16.0, "aggression": 13.0, "anticipation": 13.0, "bravery": 2.0, "composure": 8.0, "concentration": 18.0, "decisions": 15.0, "determination": 14.0, "flair": 3.0, "leadership": 2.0, "off_the_ball": 18.0, "positioning": 3.0, "teamwork": 14.0, "vision": 2.0, "work_rate": 17.0, "acceleration": 17.0, "agility": 2.0, "balance": 3.0, "jumping_reach": 18.0, "natural_fitness": 12.0, "pace": 15.0, "stamina": 7.0, "strength": 11.0}</t>
+        </is>
+      </c>
+      <c r="AC21" t="inlineStr">
+        <is>
+          <t>{"Consistency": 18.1, "Controversy": 2.5, "Dirtiness": 1.0, "Important Matches": 18.2, "Injury Proneness": 10.1, "Loyalty": 19.6, "Pressure": 16.9, "Professionalism": 18.3, "Sportsmanship": 17.1, "Temperament": 17.2, "Versatility": 14.0, "Ambition": 17.1, "Adaptability": 19.8}</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t xml:space="preserve">John </t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Cooney</t>
+        </is>
+      </c>
+      <c r="D22" s="2" t="n">
+        <v>32894</v>
+      </c>
+      <c r="E22" t="n">
+        <v>183</v>
+      </c>
+      <c r="F22" t="n">
+        <v>100</v>
+      </c>
+      <c r="G22" t="n">
+        <v>1</v>
+      </c>
+      <c r="H22" t="n">
+        <v>75</v>
+      </c>
+      <c r="I22" t="inlineStr"/>
+      <c r="J22" t="inlineStr"/>
+      <c r="K22" t="inlineStr"/>
+      <c r="L22" t="inlineStr"/>
+      <c r="M22" t="inlineStr"/>
+      <c r="N22" t="inlineStr">
+        <is>
+          <t>sh:5</t>
+        </is>
+      </c>
+      <c r="O22" t="n">
+        <v>6</v>
+      </c>
+      <c r="P22" t="inlineStr"/>
+      <c r="Q22" t="inlineStr"/>
+      <c r="R22" t="inlineStr"/>
+      <c r="S22" t="inlineStr"/>
+      <c r="T22" t="inlineStr"/>
+      <c r="U22" t="inlineStr"/>
+      <c r="V22" t="inlineStr"/>
+      <c r="W22" t="inlineStr"/>
+      <c r="X22" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y22" t="inlineStr"/>
+      <c r="Z22" t="inlineStr"/>
+      <c r="AA22" t="inlineStr"/>
+      <c r="AB22" t="inlineStr">
+        <is>
+          <t>{"darts": 3.0, "finishing": 16.0, "footwork": 18.0, "goal_kicking": 12.0, "handling": 3.0, "kicking": 10.0, "kicking_power": 8.0, "lineouts": 4.0, "marking": 5.0, "offloading": 6.0, "passing": 10.0, "scrummaging": 14.0, "rucking": 13.0, "technique": 14.0, "aggression": 14.0, "anticipation": 18.0, "bravery": 6.0, "composure": 4.0, "concentration": 2.0, "decisions": 16.0, "determination": 15.0, "flair": 18.0, "leadership": 12.0, "off_the_ball": 5.0, "positioning": 17.0, "teamwork": 9.0, "vision": 18.0, "work_rate": 3.0, "acceleration": 18.0, "agility": 9.0, "balance": 8.0, "jumping_reach": 2.0, "natural_fitness": 16.0, "pace": 3.0, "stamina": 17.0, "strength": 7.0}</t>
+        </is>
+      </c>
+      <c r="AC22" t="inlineStr">
+        <is>
+          <t>{"Consistency": 18.5, "Controversy": 1.7, "Dirtiness": 3.4, "Important Matches": 14.4, "Injury Proneness": 9.8, "Loyalty": 14.3, "Pressure": 14.3, "Professionalism": 19.9, "Sportsmanship": 18.5, "Temperament": 19.9, "Versatility": 7.8, "Ambition": 19.0, "Adaptability": 19.8}</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Ross</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Byrne</t>
+        </is>
+      </c>
+      <c r="D23" s="2" t="n">
+        <v>32895</v>
+      </c>
+      <c r="E23" t="n">
+        <v>183</v>
+      </c>
+      <c r="F23" t="n">
+        <v>100</v>
+      </c>
+      <c r="G23" t="n">
+        <v>1</v>
+      </c>
+      <c r="H23" t="n">
+        <v>75</v>
+      </c>
+      <c r="I23" t="inlineStr"/>
+      <c r="J23" t="inlineStr"/>
+      <c r="K23" t="inlineStr"/>
+      <c r="L23" t="inlineStr"/>
+      <c r="M23" t="inlineStr"/>
+      <c r="N23" t="inlineStr">
+        <is>
+          <t>fh:5</t>
+        </is>
+      </c>
+      <c r="O23" t="n">
+        <v>7</v>
+      </c>
+      <c r="P23" t="inlineStr"/>
+      <c r="Q23" t="inlineStr"/>
+      <c r="R23" t="inlineStr"/>
+      <c r="S23" t="inlineStr"/>
+      <c r="T23" t="inlineStr"/>
+      <c r="U23" t="inlineStr"/>
+      <c r="V23" t="inlineStr"/>
+      <c r="W23" t="inlineStr"/>
+      <c r="X23" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y23" t="inlineStr"/>
+      <c r="Z23" t="inlineStr"/>
+      <c r="AA23" t="inlineStr"/>
+      <c r="AB23" t="inlineStr">
+        <is>
+          <t>{"darts": 3.0, "finishing": 13.0, "footwork": 17.0, "goal_kicking": 18.0, "handling": 9.0, "kicking": 7.0, "kicking_power": 5.0, "lineouts": 1.0, "marking": 19.0, "offloading": 8.0, "passing": 13.0, "scrummaging": 10.0, "rucking": 19.0, "technique": 11.0, "aggression": 9.0, "anticipation": 13.0, "bravery": 5.0, "composure": 2.0, "concentration": 16.0, "decisions": 3.0, "determination": 16.0, "flair": 6.0, "leadership": 16.0, "off_the_ball": 12.0, "positioning": 2.0, "teamwork": 2.0, "vision": 10.0, "work_rate": 20.0, "acceleration": 2.0, "agility": 9.0, "balance": 9.0, "jumping_reach": 13.0, "natural_fitness": 16.0, "pace": 4.0, "stamina": 14.0, "strength": 15.0}</t>
+        </is>
+      </c>
+      <c r="AC23" t="inlineStr">
+        <is>
+          <t>{"Consistency": 15.4, "Controversy": 3.8, "Dirtiness": 1.3, "Important Matches": 15.6, "Injury Proneness": 3.5, "Loyalty": 16.5, "Pressure": 17.4, "Professionalism": 19.3, "Sportsmanship": 17.9, "Temperament": 19.0, "Versatility": 3.0, "Ambition": 19.0, "Adaptability": 18.7}</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Calvin</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Nash</t>
+        </is>
+      </c>
+      <c r="D24" s="2" t="n">
+        <v>32896</v>
+      </c>
+      <c r="E24" t="n">
+        <v>183</v>
+      </c>
+      <c r="F24" t="n">
+        <v>100</v>
+      </c>
+      <c r="G24" t="n">
+        <v>1</v>
+      </c>
+      <c r="H24" t="n">
+        <v>75</v>
+      </c>
+      <c r="I24" t="inlineStr"/>
+      <c r="J24" t="inlineStr"/>
+      <c r="K24" t="inlineStr"/>
+      <c r="L24" t="inlineStr"/>
+      <c r="M24" t="inlineStr"/>
+      <c r="N24" t="inlineStr">
+        <is>
+          <t>wg:5</t>
+        </is>
+      </c>
+      <c r="O24" t="n">
+        <v>9</v>
+      </c>
+      <c r="P24" t="inlineStr"/>
+      <c r="Q24" t="inlineStr"/>
+      <c r="R24" t="inlineStr"/>
+      <c r="S24" t="inlineStr"/>
+      <c r="T24" t="inlineStr"/>
+      <c r="U24" t="inlineStr"/>
+      <c r="V24" t="inlineStr"/>
+      <c r="W24" t="inlineStr"/>
+      <c r="X24" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y24" t="inlineStr"/>
+      <c r="Z24" t="inlineStr"/>
+      <c r="AA24" t="inlineStr"/>
+      <c r="AB24" t="inlineStr">
+        <is>
+          <t>{"darts": 3.0, "finishing": 18.0, "footwork": 8.0, "goal_kicking": 9.0, "handling": 3.0, "kicking": 6.0, "kicking_power": 16.0, "lineouts": 6.0, "marking": 14.0, "offloading": 2.0, "passing": 14.0, "scrummaging": 11.0, "rucking": 10.0, "technique": 14.0, "aggression": 17.0, "anticipation": 4.0, "bravery": 10.0, "composure": 19.0, "concentration": 17.0, "decisions": 17.0, "determination": 4.0, "flair": 13.0, "leadership": 3.0, "off_the_ball": 10.0, "positioning": 6.0, "teamwork": 15.0, "vision": 16.0, "work_rate": 14.0, "acceleration": 9.0, "agility": 8.0, "balance": 4.0, "jumping_reach": 9.0, "natural_fitness": 8.0, "pace": 4.0, "stamina": 14.0, "strength": 12.0}</t>
+        </is>
+      </c>
+      <c r="AC24" t="inlineStr">
+        <is>
+          <t>{"Consistency": 15.7, "Controversy": 1.8, "Dirtiness": 4.1, "Important Matches": 19.3, "Injury Proneness": 10.5, "Loyalty": 14.3, "Pressure": 18.5, "Professionalism": 19.5, "Sportsmanship": 17.9, "Temperament": 18.5, "Versatility": 3.2, "Ambition": 18.0, "Adaptability": 19.9}</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ellis </t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Genge</t>
+        </is>
+      </c>
+      <c r="D25" s="2" t="n">
+        <v>32897</v>
+      </c>
+      <c r="E25" t="n">
+        <v>183</v>
+      </c>
+      <c r="F25" t="n">
+        <v>100</v>
+      </c>
+      <c r="G25" t="n">
+        <v>2</v>
+      </c>
+      <c r="H25" t="n">
+        <v>75</v>
+      </c>
+      <c r="I25" t="inlineStr"/>
+      <c r="J25" t="inlineStr"/>
+      <c r="K25" t="inlineStr"/>
+      <c r="L25" t="inlineStr"/>
+      <c r="M25" t="inlineStr"/>
+      <c r="N25" t="inlineStr">
+        <is>
+          <t>lp:5</t>
+        </is>
+      </c>
+      <c r="O25" t="n">
+        <v>1</v>
+      </c>
+      <c r="P25" t="inlineStr"/>
+      <c r="Q25" t="inlineStr"/>
+      <c r="R25" t="inlineStr"/>
+      <c r="S25" t="inlineStr"/>
+      <c r="T25" t="inlineStr"/>
+      <c r="U25" t="inlineStr"/>
+      <c r="V25" t="inlineStr"/>
+      <c r="W25" t="inlineStr"/>
+      <c r="X25" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y25" t="inlineStr"/>
+      <c r="Z25" t="inlineStr"/>
+      <c r="AA25" t="inlineStr"/>
+      <c r="AB25" t="inlineStr">
+        <is>
+          <t>{"darts": 17.0, "finishing": 9.0, "footwork": 5.0, "goal_kicking": 5.0, "handling": 7.0, "kicking": 7.0, "kicking_power": 5.0, "lineouts": 2.0, "marking": 5.0, "offloading": 4.0, "passing": 3.0, "scrummaging": 18.0, "rucking": 11.0, "technique": 19.0, "aggression": 16.0, "anticipation": 12.0, "bravery": 3.0, "composure": 8.0, "concentration": 6.0, "decisions": 20.0, "determination": 19.0, "flair": 10.0, "leadership": 9.0, "off_the_ball": 3.0, "positioning": 9.0, "teamwork": 11.0, "vision": 15.0, "work_rate": 7.0, "acceleration": 11.0, "agility": 8.0, "balance": 17.0, "jumping_reach": 5.0, "natural_fitness": 19.0, "pace": 9.0, "stamina": 5.0, "strength": 14.0}</t>
+        </is>
+      </c>
+      <c r="AC25" t="inlineStr">
+        <is>
+          <t>{"Consistency": 20.0, "Controversy": 4.7, "Dirtiness": 1.2, "Important Matches": 15.2, "Injury Proneness": 19.0, "Loyalty": 20.0, "Pressure": 14.6, "Professionalism": 19.0, "Sportsmanship": 17.4, "Temperament": 18.4, "Versatility": 2.2, "Ambition": 19.4, "Adaptability": 17.9}</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Jamie</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>George</t>
+        </is>
+      </c>
+      <c r="D26" s="2" t="n">
+        <v>32898</v>
+      </c>
+      <c r="E26" t="n">
+        <v>183</v>
+      </c>
+      <c r="F26" t="n">
+        <v>100</v>
+      </c>
+      <c r="G26" t="n">
+        <v>2</v>
+      </c>
+      <c r="H26" t="n">
+        <v>75</v>
+      </c>
+      <c r="I26" t="inlineStr"/>
+      <c r="J26" t="inlineStr"/>
+      <c r="K26" t="inlineStr"/>
+      <c r="L26" t="inlineStr"/>
+      <c r="M26" t="inlineStr"/>
+      <c r="N26" t="inlineStr">
+        <is>
+          <t>hk:5</t>
+        </is>
+      </c>
+      <c r="O26" t="n">
+        <v>3</v>
+      </c>
+      <c r="P26" t="inlineStr"/>
+      <c r="Q26" t="inlineStr"/>
+      <c r="R26" t="inlineStr"/>
+      <c r="S26" t="inlineStr"/>
+      <c r="T26" t="inlineStr"/>
+      <c r="U26" t="inlineStr"/>
+      <c r="V26" t="inlineStr"/>
+      <c r="W26" t="inlineStr"/>
+      <c r="X26" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y26" t="inlineStr"/>
+      <c r="Z26" t="inlineStr"/>
+      <c r="AA26" t="inlineStr"/>
+      <c r="AB26" t="inlineStr">
+        <is>
+          <t>{"darts": 10.0, "finishing": 17.0, "footwork": 15.0, "goal_kicking": 5.0, "handling": 4.0, "kicking": 7.0, "kicking_power": 6.0, "lineouts": 2.0, "marking": 11.0, "offloading": 18.0, "passing": 8.0, "scrummaging": 16.0, "rucking": 5.0, "technique": 3.0, "aggression": 17.0, "anticipation": 9.0, "bravery": 17.0, "composure": 13.0, "concentration": 12.0, "decisions": 17.0, "determination": 18.0, "flair": 8.0, "leadership": 7.0, "off_the_ball": 16.0, "positioning": 8.0, "teamwork": 4.0, "vision": 17.0, "work_rate": 4.0, "acceleration": 13.0, "agility": 5.0, "balance": 3.0, "jumping_reach": 6.0, "natural_fitness": 13.0, "pace": 11.0, "stamina": 12.0, "strength": 6.0}</t>
+        </is>
+      </c>
+      <c r="AC26" t="inlineStr">
+        <is>
+          <t>{"Consistency": 14.4, "Controversy": 3.3, "Dirtiness": 2.5, "Important Matches": 16.2, "Injury Proneness": 16.6, "Loyalty": 17.9, "Pressure": 15.9, "Professionalism": 18.9, "Sportsmanship": 19.0, "Temperament": 19.3, "Versatility": 11.1, "Ambition": 19.0, "Adaptability": 18.9}</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Will  </t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Stuart  </t>
+        </is>
+      </c>
+      <c r="D27" s="2" t="n">
+        <v>32899</v>
+      </c>
+      <c r="E27" t="n">
+        <v>183</v>
+      </c>
+      <c r="F27" t="n">
+        <v>100</v>
+      </c>
+      <c r="G27" t="n">
+        <v>2</v>
+      </c>
+      <c r="H27" t="n">
+        <v>75</v>
+      </c>
+      <c r="I27" t="inlineStr"/>
+      <c r="J27" t="inlineStr"/>
+      <c r="K27" t="inlineStr"/>
+      <c r="L27" t="inlineStr"/>
+      <c r="M27" t="inlineStr"/>
+      <c r="N27" t="inlineStr">
+        <is>
+          <t>tp:5</t>
+        </is>
+      </c>
+      <c r="O27" t="n">
+        <v>2</v>
+      </c>
+      <c r="P27" t="inlineStr"/>
+      <c r="Q27" t="inlineStr"/>
+      <c r="R27" t="inlineStr"/>
+      <c r="S27" t="inlineStr"/>
+      <c r="T27" t="inlineStr"/>
+      <c r="U27" t="inlineStr"/>
+      <c r="V27" t="inlineStr"/>
+      <c r="W27" t="inlineStr"/>
+      <c r="X27" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y27" t="inlineStr"/>
+      <c r="Z27" t="inlineStr"/>
+      <c r="AA27" t="inlineStr"/>
+      <c r="AB27" t="inlineStr">
+        <is>
+          <t>{"darts": 10.0, "finishing": 11.0, "footwork": 12.0, "goal_kicking": 2.0, "handling": 12.0, "kicking": 2.0, "kicking_power": 5.0, "lineouts": 2.0, "marking": 18.0, "offloading": 19.0, "passing": 16.0, "scrummaging": 9.0, "rucking": 18.0, "technique": 17.0, "aggression": 2.0, "anticipation": 17.0, "bravery": 13.0, "composure": 10.0, "concentration": 6.0, "decisions": 20.0, "determination": 10.0, "flair": 5.0, "leadership": 12.0, "off_the_ball": 8.0, "positioning": 8.0, "teamwork": 6.0, "vision": 3.0, "work_rate": 19.0, "acceleration": 7.0, "agility": 3.0, "balance": 8.0, "jumping_reach": 2.0, "natural_fitness": 9.0, "pace": 8.0, "stamina": 19.0, "strength": 13.0}</t>
+        </is>
+      </c>
+      <c r="AC27" t="inlineStr">
+        <is>
+          <t>{"Consistency": 18.2, "Controversy": 3.7, "Dirtiness": 3.3, "Important Matches": 19.3, "Injury Proneness": 4.7, "Loyalty": 17.2, "Pressure": 18.9, "Professionalism": 18.7, "Sportsmanship": 18.8, "Temperament": 17.9, "Versatility": 15.8, "Ambition": 18.0, "Adaptability": 19.5}</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Maro  </t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Itoje  </t>
+        </is>
+      </c>
+      <c r="D28" s="2" t="n">
+        <v>32900</v>
+      </c>
+      <c r="E28" t="n">
+        <v>183</v>
+      </c>
+      <c r="F28" t="n">
+        <v>100</v>
+      </c>
+      <c r="G28" t="n">
+        <v>2</v>
+      </c>
+      <c r="H28" t="n">
+        <v>75</v>
+      </c>
+      <c r="I28" t="inlineStr"/>
+      <c r="J28" t="inlineStr"/>
+      <c r="K28" t="inlineStr"/>
+      <c r="L28" t="inlineStr"/>
+      <c r="M28" t="inlineStr"/>
+      <c r="N28" t="inlineStr">
+        <is>
+          <t>sr:5</t>
+        </is>
+      </c>
+      <c r="O28" t="n">
+        <v>4</v>
+      </c>
+      <c r="P28" t="inlineStr"/>
+      <c r="Q28" t="inlineStr"/>
+      <c r="R28" t="inlineStr"/>
+      <c r="S28" t="inlineStr"/>
+      <c r="T28" t="inlineStr"/>
+      <c r="U28" t="inlineStr"/>
+      <c r="V28" t="inlineStr"/>
+      <c r="W28" t="inlineStr"/>
+      <c r="X28" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y28" t="inlineStr"/>
+      <c r="Z28" t="inlineStr"/>
+      <c r="AA28" t="inlineStr"/>
+      <c r="AB28" t="inlineStr">
+        <is>
+          <t>{"darts": 4.0, "finishing": 12.0, "footwork": 3.0, "goal_kicking": 4.0, "handling": 18.0, "kicking": 2.0, "kicking_power": 4.0, "lineouts": 16.0, "marking": 11.0, "offloading": 15.0, "passing": 11.0, "scrummaging": 12.0, "rucking": 2.0, "technique": 6.0, "aggression": 11.0, "anticipation": 5.0, "bravery": 2.0, "composure": 4.0, "concentration": 11.0, "decisions": 14.0, "determination": 19.0, "flair": 8.0, "leadership": 5.0, "off_the_ball": 16.0, "positioning": 18.0, "teamwork": 7.0, "vision": 8.0, "work_rate": 14.0, "acceleration": 15.0, "agility": 14.0, "balance": 14.0, "jumping_reach": 7.0, "natural_fitness": 18.0, "pace": 7.0, "stamina": 7.0, "strength": 12.0}</t>
+        </is>
+      </c>
+      <c r="AC28" t="inlineStr">
+        <is>
+          <t>{"Consistency": 14.7, "Controversy": 2.2, "Dirtiness": 2.5, "Important Matches": 18.9, "Injury Proneness": 17.8, "Loyalty": 15.7, "Pressure": 18.6, "Professionalism": 18.0, "Sportsmanship": 18.7, "Temperament": 19.7, "Versatility": 3.9, "Ambition": 19.6, "Adaptability": 17.2}</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t xml:space="preserve">George  </t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Martin  </t>
+        </is>
+      </c>
+      <c r="D29" s="2" t="n">
+        <v>32901</v>
+      </c>
+      <c r="E29" t="n">
+        <v>183</v>
+      </c>
+      <c r="F29" t="n">
+        <v>100</v>
+      </c>
+      <c r="G29" t="n">
+        <v>2</v>
+      </c>
+      <c r="H29" t="n">
+        <v>75</v>
+      </c>
+      <c r="I29" t="inlineStr"/>
+      <c r="J29" t="inlineStr"/>
+      <c r="K29" t="inlineStr"/>
+      <c r="L29" t="inlineStr"/>
+      <c r="M29" t="inlineStr"/>
+      <c r="N29" t="inlineStr">
+        <is>
+          <t>sr:5</t>
+        </is>
+      </c>
+      <c r="O29" t="n">
+        <v>4</v>
+      </c>
+      <c r="P29" t="inlineStr"/>
+      <c r="Q29" t="inlineStr"/>
+      <c r="R29" t="inlineStr"/>
+      <c r="S29" t="inlineStr"/>
+      <c r="T29" t="inlineStr"/>
+      <c r="U29" t="inlineStr"/>
+      <c r="V29" t="inlineStr"/>
+      <c r="W29" t="inlineStr"/>
+      <c r="X29" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y29" t="inlineStr"/>
+      <c r="Z29" t="inlineStr"/>
+      <c r="AA29" t="inlineStr"/>
+      <c r="AB29" t="inlineStr">
+        <is>
+          <t>{"darts": 4.0, "finishing": 17.0, "footwork": 10.0, "goal_kicking": 4.0, "handling": 10.0, "kicking": 3.0, "kicking_power": 6.0, "lineouts": 20.0, "marking": 11.0, "offloading": 4.0, "passing": 8.0, "scrummaging": 15.0, "rucking": 15.0, "technique": 2.0, "aggression": 5.0, "anticipation": 4.0, "bravery": 5.0, "composure": 14.0, "concentration": 12.0, "decisions": 19.0, "determination": 19.0, "flair": 5.0, "leadership": 14.0, "off_the_ball": 9.0, "positioning": 8.0, "teamwork": 16.0, "vision": 15.0, "work_rate": 9.0, "acceleration": 19.0, "agility": 4.0, "balance": 15.0, "jumping_reach": 6.0, "natural_fitness": 4.0, "pace": 10.0, "stamina": 10.0, "strength": 6.0}</t>
+        </is>
+      </c>
+      <c r="AC29" t="inlineStr">
+        <is>
+          <t>{"Consistency": 16.1, "Controversy": 3.6, "Dirtiness": 1.9, "Important Matches": 14.1, "Injury Proneness": 17.7, "Loyalty": 19.0, "Pressure": 17.2, "Professionalism": 19.9, "Sportsmanship": 18.6, "Temperament": 18.3, "Versatility": 9.9, "Ambition": 17.8, "Adaptability": 19.4}</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tom  </t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Curry  </t>
+        </is>
+      </c>
+      <c r="D30" s="2" t="n">
+        <v>32902</v>
+      </c>
+      <c r="E30" t="n">
+        <v>183</v>
+      </c>
+      <c r="F30" t="n">
+        <v>100</v>
+      </c>
+      <c r="G30" t="n">
+        <v>2</v>
+      </c>
+      <c r="H30" t="n">
+        <v>75</v>
+      </c>
+      <c r="I30" t="inlineStr"/>
+      <c r="J30" t="inlineStr"/>
+      <c r="K30" t="inlineStr"/>
+      <c r="L30" t="inlineStr"/>
+      <c r="M30" t="inlineStr"/>
+      <c r="N30" t="inlineStr">
+        <is>
+          <t>br:5</t>
+        </is>
+      </c>
+      <c r="O30" t="n">
+        <v>5</v>
+      </c>
+      <c r="P30" t="inlineStr"/>
+      <c r="Q30" t="inlineStr"/>
+      <c r="R30" t="inlineStr"/>
+      <c r="S30" t="inlineStr"/>
+      <c r="T30" t="inlineStr"/>
+      <c r="U30" t="inlineStr"/>
+      <c r="V30" t="inlineStr"/>
+      <c r="W30" t="inlineStr"/>
+      <c r="X30" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y30" t="inlineStr"/>
+      <c r="Z30" t="inlineStr"/>
+      <c r="AA30" t="inlineStr"/>
+      <c r="AB30" t="inlineStr">
+        <is>
+          <t>{"darts": 13.0, "finishing": 6.0, "footwork": 5.0, "goal_kicking": 4.0, "handling": 6.0, "kicking": 9.0, "kicking_power": 8.0, "lineouts": 10.0, "marking": 7.0, "offloading": 8.0, "passing": 5.0, "scrummaging": 3.0, "rucking": 12.0, "technique": 9.0, "aggression": 20.0, "anticipation": 15.0, "bravery": 19.0, "composure": 7.0, "concentration": 14.0, "decisions": 19.0, "determination": 14.0, "flair": 10.0, "leadership": 10.0, "off_the_ball": 15.0, "positioning": 14.0, "teamwork": 7.0, "vision": 19.0, "work_rate": 6.0, "acceleration": 11.0, "agility": 4.0, "balance": 6.0, "jumping_reach": 17.0, "natural_fitness": 6.0, "pace": 3.0, "stamina": 19.0, "strength": 9.0}</t>
+        </is>
+      </c>
+      <c r="AC30" t="inlineStr">
+        <is>
+          <t>{"Consistency": 19.0, "Controversy": 2.7, "Dirtiness": 1.4, "Important Matches": 20.0, "Injury Proneness": 16.0, "Loyalty": 15.0, "Pressure": 17.0, "Professionalism": 19.1, "Sportsmanship": 17.6, "Temperament": 19.8, "Versatility": 15.3, "Ambition": 17.1, "Adaptability": 17.7}</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ben  </t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Curry  </t>
+        </is>
+      </c>
+      <c r="D31" s="2" t="n">
+        <v>32903</v>
+      </c>
+      <c r="E31" t="n">
+        <v>183</v>
+      </c>
+      <c r="F31" t="n">
+        <v>100</v>
+      </c>
+      <c r="G31" t="n">
+        <v>2</v>
+      </c>
+      <c r="H31" t="n">
+        <v>75</v>
+      </c>
+      <c r="I31" t="inlineStr"/>
+      <c r="J31" t="inlineStr"/>
+      <c r="K31" t="inlineStr"/>
+      <c r="L31" t="inlineStr"/>
+      <c r="M31" t="inlineStr"/>
+      <c r="N31" t="inlineStr">
+        <is>
+          <t>br:5</t>
+        </is>
+      </c>
+      <c r="O31" t="n">
+        <v>5</v>
+      </c>
+      <c r="P31" t="inlineStr"/>
+      <c r="Q31" t="inlineStr"/>
+      <c r="R31" t="inlineStr"/>
+      <c r="S31" t="inlineStr"/>
+      <c r="T31" t="inlineStr"/>
+      <c r="U31" t="inlineStr"/>
+      <c r="V31" t="inlineStr"/>
+      <c r="W31" t="inlineStr"/>
+      <c r="X31" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y31" t="inlineStr"/>
+      <c r="Z31" t="inlineStr"/>
+      <c r="AA31" t="inlineStr"/>
+      <c r="AB31" t="inlineStr">
+        <is>
+          <t>{"darts": 11.0, "finishing": 15.0, "footwork": 19.0, "goal_kicking": 2.0, "handling": 2.0, "kicking": 6.0, "kicking_power": 3.0, "lineouts": 20.0, "marking": 6.0, "offloading": 16.0, "passing": 15.0, "scrummaging": 16.0, "rucking": 18.0, "technique": 3.0, "aggression": 14.0, "anticipation": 2.0, "bravery": 6.0, "composure": 20.0, "concentration": 8.0, "decisions": 19.0, "determination": 16.0, "flair": 12.0, "leadership": 2.0, "off_the_ball": 1.0, "positioning": 4.0, "teamwork": 8.0, "vision": 6.0, "work_rate": 12.0, "acceleration": 3.0, "agility": 17.0, "balance": 16.0, "jumping_reach": 17.0, "natural_fitness": 12.0, "pace": 2.0, "stamina": 1.0, "strength": 5.0}</t>
+        </is>
+      </c>
+      <c r="AC31" t="inlineStr">
+        <is>
+          <t>{"Consistency": 16.5, "Controversy": 4.6, "Dirtiness": 4.3, "Important Matches": 19.6, "Injury Proneness": 8.9, "Loyalty": 15.9, "Pressure": 15.6, "Professionalism": 18.2, "Sportsmanship": 19.6, "Temperament": 19.5, "Versatility": 14.0, "Ambition": 17.7, "Adaptability": 17.5}</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ben  </t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Earl  </t>
+        </is>
+      </c>
+      <c r="D32" s="2" t="n">
+        <v>32904</v>
+      </c>
+      <c r="E32" t="n">
+        <v>183</v>
+      </c>
+      <c r="F32" t="n">
+        <v>100</v>
+      </c>
+      <c r="G32" t="n">
+        <v>2</v>
+      </c>
+      <c r="H32" t="n">
+        <v>75</v>
+      </c>
+      <c r="I32" t="inlineStr"/>
+      <c r="J32" t="inlineStr"/>
+      <c r="K32" t="inlineStr"/>
+      <c r="L32" t="inlineStr"/>
+      <c r="M32" t="inlineStr"/>
+      <c r="N32" t="inlineStr">
+        <is>
+          <t>br:5</t>
+        </is>
+      </c>
+      <c r="O32" t="n">
+        <v>5</v>
+      </c>
+      <c r="P32" t="inlineStr"/>
+      <c r="Q32" t="inlineStr"/>
+      <c r="R32" t="inlineStr"/>
+      <c r="S32" t="inlineStr"/>
+      <c r="T32" t="inlineStr"/>
+      <c r="U32" t="inlineStr"/>
+      <c r="V32" t="inlineStr"/>
+      <c r="W32" t="inlineStr"/>
+      <c r="X32" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y32" t="inlineStr"/>
+      <c r="Z32" t="inlineStr"/>
+      <c r="AA32" t="inlineStr"/>
+      <c r="AB32" t="inlineStr">
+        <is>
+          <t>{"darts": 2.0, "finishing": 13.0, "footwork": 17.0, "goal_kicking": 4.0, "handling": 13.0, "kicking": 3.0, "kicking_power": 9.0, "lineouts": 8.0, "marking": 18.0, "offloading": 2.0, "passing": 13.0, "scrummaging": 7.0, "rucking": 11.0, "technique": 8.0, "aggression": 11.0, "anticipation": 19.0, "bravery": 12.0, "composure": 11.0, "concentration": 12.0, "decisions": 10.0, "determination": 8.0, "flair": 4.0, "leadership": 2.0, "off_the_ball": 11.0, "positioning": 5.0, "teamwork": 5.0, "vision": 14.0, "work_rate": 14.0, "acceleration": 17.0, "agility": 10.0, "balance": 19.0, "jumping_reach": 8.0, "natural_fitness": 1.0, "pace": 15.0, "stamina": 5.0, "strength": 17.0}</t>
+        </is>
+      </c>
+      <c r="AC32" t="inlineStr">
+        <is>
+          <t>{"Consistency": 14.6, "Controversy": 3.0, "Dirtiness": 1.8, "Important Matches": 19.7, "Injury Proneness": 14.2, "Loyalty": 17.2, "Pressure": 14.6, "Professionalism": 18.4, "Sportsmanship": 18.0, "Temperament": 18.0, "Versatility": 2.2, "Ambition": 17.1, "Adaptability": 18.9}</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Alex  </t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mitchell  </t>
+        </is>
+      </c>
+      <c r="D33" s="2" t="n">
+        <v>32905</v>
+      </c>
+      <c r="E33" t="n">
+        <v>183</v>
+      </c>
+      <c r="F33" t="n">
+        <v>100</v>
+      </c>
+      <c r="G33" t="n">
+        <v>2</v>
+      </c>
+      <c r="H33" t="n">
+        <v>75</v>
+      </c>
+      <c r="I33" t="inlineStr"/>
+      <c r="J33" t="inlineStr"/>
+      <c r="K33" t="inlineStr"/>
+      <c r="L33" t="inlineStr"/>
+      <c r="M33" t="inlineStr"/>
+      <c r="N33" t="inlineStr">
+        <is>
+          <t>sh:5</t>
+        </is>
+      </c>
+      <c r="O33" t="n">
+        <v>6</v>
+      </c>
+      <c r="P33" t="inlineStr"/>
+      <c r="Q33" t="inlineStr"/>
+      <c r="R33" t="inlineStr"/>
+      <c r="S33" t="inlineStr"/>
+      <c r="T33" t="inlineStr"/>
+      <c r="U33" t="inlineStr"/>
+      <c r="V33" t="inlineStr"/>
+      <c r="W33" t="inlineStr"/>
+      <c r="X33" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y33" t="inlineStr"/>
+      <c r="Z33" t="inlineStr"/>
+      <c r="AA33" t="inlineStr"/>
+      <c r="AB33" t="inlineStr">
+        <is>
+          <t>{"darts": 5.0, "finishing": 16.0, "footwork": 4.0, "goal_kicking": 16.0, "handling": 3.0, "kicking": 5.0, "kicking_power": 12.0, "lineouts": 8.0, "marking": 9.0, "offloading": 14.0, "passing": 12.0, "scrummaging": 14.0, "rucking": 1.0, "technique": 10.0, "aggression": 13.0, "anticipation": 9.0, "bravery": 17.0, "composure": 14.0, "concentration": 13.0, "decisions": 8.0, "determination": 16.0, "flair": 15.0, "leadership": 7.0, "off_the_ball": 2.0, "positioning": 5.0, "teamwork": 16.0, "vision": 18.0, "work_rate": 3.0, "acceleration": 15.0, "agility": 2.0, "balance": 19.0, "jumping_reach": 4.0, "natural_fitness": 3.0, "pace": 12.0, "stamina": 11.0, "strength": 10.0}</t>
+        </is>
+      </c>
+      <c r="AC33" t="inlineStr">
+        <is>
+          <t>{"Consistency": 14.6, "Controversy": 4.3, "Dirtiness": 1.1, "Important Matches": 18.5, "Injury Proneness": 1.5, "Loyalty": 16.7, "Pressure": 15.0, "Professionalism": 18.3, "Sportsmanship": 18.2, "Temperament": 19.8, "Versatility": 9.4, "Ambition": 17.0, "Adaptability": 19.9}</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Marcus  </t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Smith  </t>
+        </is>
+      </c>
+      <c r="D34" s="2" t="n">
+        <v>32906</v>
+      </c>
+      <c r="E34" t="n">
+        <v>183</v>
+      </c>
+      <c r="F34" t="n">
+        <v>100</v>
+      </c>
+      <c r="G34" t="n">
+        <v>2</v>
+      </c>
+      <c r="H34" t="n">
+        <v>75</v>
+      </c>
+      <c r="I34" t="inlineStr"/>
+      <c r="J34" t="inlineStr"/>
+      <c r="K34" t="inlineStr"/>
+      <c r="L34" t="inlineStr"/>
+      <c r="M34" t="inlineStr"/>
+      <c r="N34" t="inlineStr">
+        <is>
+          <t>fh:5</t>
+        </is>
+      </c>
+      <c r="O34" t="n">
+        <v>7</v>
+      </c>
+      <c r="P34" t="inlineStr"/>
+      <c r="Q34" t="inlineStr"/>
+      <c r="R34" t="inlineStr"/>
+      <c r="S34" t="inlineStr"/>
+      <c r="T34" t="inlineStr"/>
+      <c r="U34" t="inlineStr"/>
+      <c r="V34" t="inlineStr"/>
+      <c r="W34" t="inlineStr"/>
+      <c r="X34" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y34" t="inlineStr"/>
+      <c r="Z34" t="inlineStr"/>
+      <c r="AA34" t="inlineStr"/>
+      <c r="AB34" t="inlineStr">
+        <is>
+          <t>{"darts": 5.0, "finishing": 12.0, "footwork": 8.0, "goal_kicking": 9.0, "handling": 5.0, "kicking": 11.0, "kicking_power": 7.0, "lineouts": 5.0, "marking": 9.0, "offloading": 6.0, "passing": 4.0, "scrummaging": 5.0, "rucking": 3.0, "technique": 8.0, "aggression": 19.0, "anticipation": 9.0, "bravery": 8.0, "composure": 10.0, "concentration": 12.0, "decisions": 6.0, "determination": 12.0, "flair": 8.0, "leadership": 10.0, "off_the_ball": 10.0, "positioning": 14.0, "teamwork": 8.0, "vision": 16.0, "work_rate": 7.0, "acceleration": 20.0, "agility": 17.0, "balance": 12.0, "jumping_reach": 3.0, "natural_fitness": 18.0, "pace": 15.0, "stamina": 16.0, "strength": 15.0}</t>
+        </is>
+      </c>
+      <c r="AC34" t="inlineStr">
+        <is>
+          <t>{"Consistency": 18.8, "Controversy": 4.3, "Dirtiness": 1.6, "Important Matches": 18.4, "Injury Proneness": 11.8, "Loyalty": 18.2, "Pressure": 16.7, "Professionalism": 18.4, "Sportsmanship": 19.9, "Temperament": 18.3, "Versatility": 14.3, "Ambition": 18.7, "Adaptability": 18.9}</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cadan  </t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Murley  </t>
+        </is>
+      </c>
+      <c r="D35" s="2" t="n">
+        <v>32907</v>
+      </c>
+      <c r="E35" t="n">
+        <v>183</v>
+      </c>
+      <c r="F35" t="n">
+        <v>100</v>
+      </c>
+      <c r="G35" t="n">
+        <v>2</v>
+      </c>
+      <c r="H35" t="n">
+        <v>75</v>
+      </c>
+      <c r="I35" t="inlineStr"/>
+      <c r="J35" t="inlineStr"/>
+      <c r="K35" t="inlineStr"/>
+      <c r="L35" t="inlineStr"/>
+      <c r="M35" t="inlineStr"/>
+      <c r="N35" t="inlineStr">
+        <is>
+          <t>wg:5</t>
+        </is>
+      </c>
+      <c r="O35" t="n">
+        <v>9</v>
+      </c>
+      <c r="P35" t="inlineStr"/>
+      <c r="Q35" t="inlineStr"/>
+      <c r="R35" t="inlineStr"/>
+      <c r="S35" t="inlineStr"/>
+      <c r="T35" t="inlineStr"/>
+      <c r="U35" t="inlineStr"/>
+      <c r="V35" t="inlineStr"/>
+      <c r="W35" t="inlineStr"/>
+      <c r="X35" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y35" t="inlineStr"/>
+      <c r="Z35" t="inlineStr"/>
+      <c r="AA35" t="inlineStr"/>
+      <c r="AB35" t="inlineStr">
+        <is>
+          <t>{"darts": 4.0, "finishing": 19.0, "footwork": 12.0, "goal_kicking": 15.0, "handling": 18.0, "kicking": 9.0, "kicking_power": 4.0, "lineouts": 1.0, "marking": 12.0, "offloading": 5.0, "passing": 3.0, "scrummaging": 16.0, "rucking": 18.0, "technique": 13.0, "aggression": 5.0, "anticipation": 12.0, "bravery": 11.0, "composure": 15.0, "concentration": 18.0, "decisions": 13.0, "determination": 2.0, "flair": 9.0, "leadership": 13.0, "off_the_ball": 3.0, "positioning": 19.0, "teamwork": 6.0, "vision": 20.0, "work_rate": 2.0, "acceleration": 6.0, "agility": 15.0, "balance": 7.0, "jumping_reach": 11.0, "natural_fitness": 14.0, "pace": 13.0, "stamina": 9.0, "strength": 6.0}</t>
+        </is>
+      </c>
+      <c r="AC35" t="inlineStr">
+        <is>
+          <t>{"Consistency": 18.5, "Controversy": 3.9, "Dirtiness": 1.9, "Important Matches": 16.4, "Injury Proneness": 7.5, "Loyalty": 19.2, "Pressure": 17.2, "Professionalism": 18.1, "Sportsmanship": 18.5, "Temperament": 17.3, "Versatility": 15.7, "Ambition": 19.6, "Adaptability": 18.8}</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Henry  </t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Slade  </t>
+        </is>
+      </c>
+      <c r="D36" s="2" t="n">
+        <v>32908</v>
+      </c>
+      <c r="E36" t="n">
+        <v>183</v>
+      </c>
+      <c r="F36" t="n">
+        <v>100</v>
+      </c>
+      <c r="G36" t="n">
+        <v>2</v>
+      </c>
+      <c r="H36" t="n">
+        <v>75</v>
+      </c>
+      <c r="I36" t="inlineStr"/>
+      <c r="J36" t="inlineStr"/>
+      <c r="K36" t="inlineStr"/>
+      <c r="L36" t="inlineStr"/>
+      <c r="M36" t="inlineStr"/>
+      <c r="N36" t="inlineStr">
+        <is>
+          <t>ct:5</t>
+        </is>
+      </c>
+      <c r="O36" t="n">
+        <v>8</v>
+      </c>
+      <c r="P36" t="inlineStr"/>
+      <c r="Q36" t="inlineStr"/>
+      <c r="R36" t="inlineStr"/>
+      <c r="S36" t="inlineStr"/>
+      <c r="T36" t="inlineStr"/>
+      <c r="U36" t="inlineStr"/>
+      <c r="V36" t="inlineStr"/>
+      <c r="W36" t="inlineStr"/>
+      <c r="X36" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y36" t="inlineStr"/>
+      <c r="Z36" t="inlineStr"/>
+      <c r="AA36" t="inlineStr"/>
+      <c r="AB36" t="inlineStr">
+        <is>
+          <t>{"darts": 2.0, "finishing": 13.0, "footwork": 8.0, "goal_kicking": 10.0, "handling": 20.0, "kicking": 16.0, "kicking_power": 15.0, "lineouts": 3.0, "marking": 9.0, "offloading": 7.0, "passing": 3.0, "scrummaging": 19.0, "rucking": 9.0, "technique": 5.0, "aggression": 18.0, "anticipation": 4.0, "bravery": 8.0, "composure": 3.0, "concentration": 20.0, "decisions": 19.0, "determination": 9.0, "flair": 5.0, "leadership": 9.0, "off_the_ball": 20.0, "positioning": 7.0, "teamwork": 2.0, "vision": 10.0, "work_rate": 11.0, "acceleration": 4.0, "agility": 19.0, "balance": 5.0, "jumping_reach": 4.0, "natural_fitness": 19.0, "pace": 13.0, "stamina": 7.0, "strength": 6.0}</t>
+        </is>
+      </c>
+      <c r="AC36" t="inlineStr">
+        <is>
+          <t>{"Consistency": 14.1, "Controversy": 2.8, "Dirtiness": 2.4, "Important Matches": 18.0, "Injury Proneness": 10.6, "Loyalty": 15.3, "Pressure": 17.9, "Professionalism": 19.2, "Sportsmanship": 19.5, "Temperament": 19.8, "Versatility": 7.7, "Ambition": 18.5, "Adaptability": 18.4}</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ollie  </t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Lawrence  </t>
+        </is>
+      </c>
+      <c r="D37" s="2" t="n">
+        <v>32909</v>
+      </c>
+      <c r="E37" t="n">
+        <v>183</v>
+      </c>
+      <c r="F37" t="n">
+        <v>100</v>
+      </c>
+      <c r="G37" t="n">
+        <v>2</v>
+      </c>
+      <c r="H37" t="n">
+        <v>75</v>
+      </c>
+      <c r="I37" t="inlineStr"/>
+      <c r="J37" t="inlineStr"/>
+      <c r="K37" t="inlineStr"/>
+      <c r="L37" t="inlineStr"/>
+      <c r="M37" t="inlineStr"/>
+      <c r="N37" t="inlineStr">
+        <is>
+          <t>ct:5</t>
+        </is>
+      </c>
+      <c r="O37" t="n">
+        <v>8</v>
+      </c>
+      <c r="P37" t="inlineStr"/>
+      <c r="Q37" t="inlineStr"/>
+      <c r="R37" t="inlineStr"/>
+      <c r="S37" t="inlineStr"/>
+      <c r="T37" t="inlineStr"/>
+      <c r="U37" t="inlineStr"/>
+      <c r="V37" t="inlineStr"/>
+      <c r="W37" t="inlineStr"/>
+      <c r="X37" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y37" t="inlineStr"/>
+      <c r="Z37" t="inlineStr"/>
+      <c r="AA37" t="inlineStr"/>
+      <c r="AB37" t="inlineStr">
+        <is>
+          <t>{"darts": 4.0, "finishing": 12.0, "footwork": 8.0, "goal_kicking": 18.0, "handling": 14.0, "kicking": 7.0, "kicking_power": 7.0, "lineouts": 7.0, "marking": 17.0, "offloading": 6.0, "passing": 17.0, "scrummaging": 18.0, "rucking": 5.0, "technique": 6.0, "aggression": 7.0, "anticipation": 8.0, "bravery": 10.0, "composure": 8.0, "concentration": 9.0, "decisions": 2.0, "determination": 17.0, "flair": 2.0, "leadership": 2.0, "off_the_ball": 2.0, "positioning": 8.0, "teamwork": 2.0, "vision": 7.0, "work_rate": 18.0, "acceleration": 2.0, "agility": 20.0, "balance": 8.0, "jumping_reach": 16.0, "natural_fitness": 20.0, "pace": 16.0, "stamina": 8.0, "strength": 11.0}</t>
+        </is>
+      </c>
+      <c r="AC37" t="inlineStr">
+        <is>
+          <t>{"Consistency": 17.2, "Controversy": 4.0, "Dirtiness": 1.2, "Important Matches": 15.6, "Injury Proneness": 11.5, "Loyalty": 17.4, "Pressure": 14.8, "Professionalism": 19.9, "Sportsmanship": 18.5, "Temperament": 19.9, "Versatility": 17.7, "Ambition": 17.3, "Adaptability": 19.1}</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tommy  </t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Freeman  </t>
+        </is>
+      </c>
+      <c r="D38" s="2" t="n">
+        <v>32910</v>
+      </c>
+      <c r="E38" t="n">
+        <v>183</v>
+      </c>
+      <c r="F38" t="n">
+        <v>100</v>
+      </c>
+      <c r="G38" t="n">
+        <v>2</v>
+      </c>
+      <c r="H38" t="n">
+        <v>75</v>
+      </c>
+      <c r="I38" t="inlineStr"/>
+      <c r="J38" t="inlineStr"/>
+      <c r="K38" t="inlineStr"/>
+      <c r="L38" t="inlineStr"/>
+      <c r="M38" t="inlineStr"/>
+      <c r="N38" t="inlineStr">
+        <is>
+          <t>wg:5</t>
+        </is>
+      </c>
+      <c r="O38" t="n">
+        <v>9</v>
+      </c>
+      <c r="P38" t="inlineStr"/>
+      <c r="Q38" t="inlineStr"/>
+      <c r="R38" t="inlineStr"/>
+      <c r="S38" t="inlineStr"/>
+      <c r="T38" t="inlineStr"/>
+      <c r="U38" t="inlineStr"/>
+      <c r="V38" t="inlineStr"/>
+      <c r="W38" t="inlineStr"/>
+      <c r="X38" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y38" t="inlineStr"/>
+      <c r="Z38" t="inlineStr"/>
+      <c r="AA38" t="inlineStr"/>
+      <c r="AB38" t="inlineStr">
+        <is>
+          <t>{"darts": 3.0, "finishing": 15.0, "footwork": 7.0, "goal_kicking": 7.0, "handling": 8.0, "kicking": 19.0, "kicking_power": 12.0, "lineouts": 5.0, "marking": 6.0, "offloading": 12.0, "passing": 18.0, "scrummaging": 4.0, "rucking": 3.0, "technique": 18.0, "aggression": 6.0, "anticipation": 7.0, "bravery": 6.0, "composure": 5.0, "concentration": 4.0, "decisions": 7.0, "determination": 19.0, "flair": 19.0, "leadership": 17.0, "off_the_ball": 12.0, "positioning": 10.0, "teamwork": 9.0, "vision": 13.0, "work_rate": 6.0, "acceleration": 18.0, "agility": 7.0, "balance": 5.0, "jumping_reach": 9.0, "natural_fitness": 15.0, "pace": 18.0, "stamina": 13.0, "strength": 11.0}</t>
+        </is>
+      </c>
+      <c r="AC38" t="inlineStr">
+        <is>
+          <t>{"Consistency": 18.4, "Controversy": 4.9, "Dirtiness": 1.9, "Important Matches": 19.2, "Injury Proneness": 5.5, "Loyalty": 15.6, "Pressure": 16.9, "Professionalism": 19.0, "Sportsmanship": 19.5, "Temperament": 18.5, "Versatility": 5.0, "Ambition": 19.9, "Adaptability": 19.0}</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Freddie  </t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Steward  </t>
+        </is>
+      </c>
+      <c r="D39" s="2" t="n">
+        <v>32911</v>
+      </c>
+      <c r="E39" t="n">
+        <v>183</v>
+      </c>
+      <c r="F39" t="n">
+        <v>100</v>
+      </c>
+      <c r="G39" t="n">
+        <v>2</v>
+      </c>
+      <c r="H39" t="n">
+        <v>75</v>
+      </c>
+      <c r="I39" t="inlineStr"/>
+      <c r="J39" t="inlineStr"/>
+      <c r="K39" t="inlineStr"/>
+      <c r="L39" t="inlineStr"/>
+      <c r="M39" t="inlineStr"/>
+      <c r="N39" t="inlineStr">
+        <is>
+          <t>fb:5</t>
+        </is>
+      </c>
+      <c r="O39" t="n">
+        <v>10</v>
+      </c>
+      <c r="P39" t="inlineStr"/>
+      <c r="Q39" t="inlineStr"/>
+      <c r="R39" t="inlineStr"/>
+      <c r="S39" t="inlineStr"/>
+      <c r="T39" t="inlineStr"/>
+      <c r="U39" t="inlineStr"/>
+      <c r="V39" t="inlineStr"/>
+      <c r="W39" t="inlineStr"/>
+      <c r="X39" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y39" t="inlineStr"/>
+      <c r="Z39" t="inlineStr"/>
+      <c r="AA39" t="inlineStr"/>
+      <c r="AB39" t="inlineStr">
+        <is>
+          <t>{"darts": 5.0, "finishing": 7.0, "footwork": 9.0, "goal_kicking": 2.0, "handling": 18.0, "kicking": 15.0, "kicking_power": 16.0, "lineouts": 5.0, "marking": 8.0, "offloading": 5.0, "passing": 16.0, "scrummaging": 3.0, "rucking": 14.0, "technique": 14.0, "aggression": 15.0, "anticipation": 9.0, "bravery": 10.0, "composure": 2.0, "concentration": 7.0, "decisions": 12.0, "determination": 15.0, "flair": 4.0, "leadership": 18.0, "off_the_ball": 14.0, "positioning": 7.0, "teamwork": 7.0, "vision": 10.0, "work_rate": 8.0, "acceleration": 7.0, "agility": 5.0, "balance": 7.0, "jumping_reach": 6.0, "natural_fitness": 8.0, "pace": 16.0, "stamina": 20.0, "strength": 20.0}</t>
+        </is>
+      </c>
+      <c r="AC39" t="inlineStr">
+        <is>
+          <t>{"Consistency": 16.1, "Controversy": 1.2, "Dirtiness": 2.7, "Important Matches": 16.2, "Injury Proneness": 4.2, "Loyalty": 19.8, "Pressure": 15.5, "Professionalism": 18.5, "Sportsmanship": 18.6, "Temperament": 17.6, "Versatility": 3.4, "Ambition": 19.6, "Adaptability": 19.3}</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Theo  </t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Dan  </t>
+        </is>
+      </c>
+      <c r="D40" s="2" t="n">
+        <v>32912</v>
+      </c>
+      <c r="E40" t="n">
+        <v>183</v>
+      </c>
+      <c r="F40" t="n">
+        <v>100</v>
+      </c>
+      <c r="G40" t="n">
+        <v>2</v>
+      </c>
+      <c r="H40" t="n">
+        <v>75</v>
+      </c>
+      <c r="I40" t="inlineStr"/>
+      <c r="J40" t="inlineStr"/>
+      <c r="K40" t="inlineStr"/>
+      <c r="L40" t="inlineStr"/>
+      <c r="M40" t="inlineStr"/>
+      <c r="N40" t="inlineStr">
+        <is>
+          <t>hk:5</t>
+        </is>
+      </c>
+      <c r="O40" t="n">
+        <v>3</v>
+      </c>
+      <c r="P40" t="inlineStr"/>
+      <c r="Q40" t="inlineStr"/>
+      <c r="R40" t="inlineStr"/>
+      <c r="S40" t="inlineStr"/>
+      <c r="T40" t="inlineStr"/>
+      <c r="U40" t="inlineStr"/>
+      <c r="V40" t="inlineStr"/>
+      <c r="W40" t="inlineStr"/>
+      <c r="X40" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y40" t="inlineStr"/>
+      <c r="Z40" t="inlineStr"/>
+      <c r="AA40" t="inlineStr"/>
+      <c r="AB40" t="inlineStr">
+        <is>
+          <t>{"darts": 15.0, "finishing": 13.0, "footwork": 6.0, "goal_kicking": 3.0, "handling": 16.0, "kicking": 1.0, "kicking_power": 4.0, "lineouts": 8.0, "marking": 4.0, "offloading": 8.0, "passing": 16.0, "scrummaging": 18.0, "rucking": 7.0, "technique": 16.0, "aggression": 13.0, "anticipation": 2.0, "bravery": 6.0, "composure": 9.0, "concentration": 18.0, "decisions": 7.0, "determination": 11.0, "flair": 18.0, "leadership": 18.0, "off_the_ball": 8.0, "positioning": 8.0, "teamwork": 6.0, "vision": 7.0, "work_rate": 7.0, "acceleration": 15.0, "agility": 9.0, "balance": 10.0, "jumping_reach": 1.0, "natural_fitness": 7.0, "pace": 6.0, "stamina": 10.0, "strength": 20.0}</t>
+        </is>
+      </c>
+      <c r="AC40" t="inlineStr">
+        <is>
+          <t>{"Consistency": 15.5, "Controversy": 4.5, "Dirtiness": 2.3, "Important Matches": 18.9, "Injury Proneness": 13.4, "Loyalty": 14.9, "Pressure": 15.4, "Professionalism": 18.2, "Sportsmanship": 18.1, "Temperament": 19.5, "Versatility": 11.9, "Ambition": 18.5, "Adaptability": 19.2}</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fin  </t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Baxter  </t>
+        </is>
+      </c>
+      <c r="D41" s="2" t="n">
+        <v>32913</v>
+      </c>
+      <c r="E41" t="n">
+        <v>183</v>
+      </c>
+      <c r="F41" t="n">
+        <v>100</v>
+      </c>
+      <c r="G41" t="n">
+        <v>2</v>
+      </c>
+      <c r="H41" t="n">
+        <v>75</v>
+      </c>
+      <c r="I41" t="inlineStr"/>
+      <c r="J41" t="inlineStr"/>
+      <c r="K41" t="inlineStr"/>
+      <c r="L41" t="inlineStr"/>
+      <c r="M41" t="inlineStr"/>
+      <c r="N41" t="inlineStr">
+        <is>
+          <t>lp:5</t>
+        </is>
+      </c>
+      <c r="O41" t="n">
+        <v>1</v>
+      </c>
+      <c r="P41" t="inlineStr"/>
+      <c r="Q41" t="inlineStr"/>
+      <c r="R41" t="inlineStr"/>
+      <c r="S41" t="inlineStr"/>
+      <c r="T41" t="inlineStr"/>
+      <c r="U41" t="inlineStr"/>
+      <c r="V41" t="inlineStr"/>
+      <c r="W41" t="inlineStr"/>
+      <c r="X41" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y41" t="inlineStr"/>
+      <c r="Z41" t="inlineStr"/>
+      <c r="AA41" t="inlineStr"/>
+      <c r="AB41" t="inlineStr">
+        <is>
+          <t>{"darts": 14.0, "finishing": 11.0, "footwork": 5.0, "goal_kicking": 5.0, "handling": 12.0, "kicking": 6.0, "kicking_power": 7.0, "lineouts": 3.0, "marking": 10.0, "offloading": 18.0, "passing": 5.0, "scrummaging": 5.0, "rucking": 19.0, "technique": 12.0, "aggression": 3.0, "anticipation": 15.0, "bravery": 13.0, "composure": 8.0, "concentration": 15.0, "decisions": 5.0, "determination": 8.0, "flair": 17.0, "leadership": 12.0, "off_the_ball": 3.0, "positioning": 11.0, "teamwork": 4.0, "vision": 20.0, "work_rate": 13.0, "acceleration": 12.0, "agility": 10.0, "balance": 11.0, "jumping_reach": 4.0, "natural_fitness": 19.0, "pace": 2.0, "stamina": 19.0, "strength": 16.0}</t>
+        </is>
+      </c>
+      <c r="AC41" t="inlineStr">
+        <is>
+          <t>{"Consistency": 15.6, "Controversy": 3.1, "Dirtiness": 3.5, "Important Matches": 16.1, "Injury Proneness": 19.5, "Loyalty": 17.1, "Pressure": 16.1, "Professionalism": 18.0, "Sportsmanship": 18.0, "Temperament": 19.8, "Versatility": 18.6, "Ambition": 19.0, "Adaptability": 18.2}</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Joe  </t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Heyes  </t>
+        </is>
+      </c>
+      <c r="D42" s="2" t="n">
+        <v>32914</v>
+      </c>
+      <c r="E42" t="n">
+        <v>183</v>
+      </c>
+      <c r="F42" t="n">
+        <v>100</v>
+      </c>
+      <c r="G42" t="n">
+        <v>2</v>
+      </c>
+      <c r="H42" t="n">
+        <v>75</v>
+      </c>
+      <c r="I42" t="inlineStr"/>
+      <c r="J42" t="inlineStr"/>
+      <c r="K42" t="inlineStr"/>
+      <c r="L42" t="inlineStr"/>
+      <c r="M42" t="inlineStr"/>
+      <c r="N42" t="inlineStr">
+        <is>
+          <t>tp:5</t>
+        </is>
+      </c>
+      <c r="O42" t="n">
+        <v>2</v>
+      </c>
+      <c r="P42" t="inlineStr"/>
+      <c r="Q42" t="inlineStr"/>
+      <c r="R42" t="inlineStr"/>
+      <c r="S42" t="inlineStr"/>
+      <c r="T42" t="inlineStr"/>
+      <c r="U42" t="inlineStr"/>
+      <c r="V42" t="inlineStr"/>
+      <c r="W42" t="inlineStr"/>
+      <c r="X42" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y42" t="inlineStr"/>
+      <c r="Z42" t="inlineStr"/>
+      <c r="AA42" t="inlineStr"/>
+      <c r="AB42" t="inlineStr">
+        <is>
+          <t>{"darts": 5.0, "finishing": 6.0, "footwork": 12.0, "goal_kicking": 5.0, "handling": 16.0, "kicking": 5.0, "kicking_power": 6.0, "lineouts": 2.0, "marking": 19.0, "offloading": 15.0, "passing": 15.0, "scrummaging": 12.0, "rucking": 15.0, "technique": 10.0, "aggression": 9.0, "anticipation": 16.0, "bravery": 12.0, "composure": 10.0, "concentration": 13.0, "decisions": 3.0, "determination": 17.0, "flair": 10.0, "leadership": 7.0, "off_the_ball": 16.0, "positioning": 6.0, "teamwork": 5.0, "vision": 17.0, "work_rate": 4.0, "acceleration": 12.0, "agility": 12.0, "balance": 19.0, "jumping_reach": 5.0, "natural_fitness": 7.0, "pace": 4.0, "stamina": 14.0, "strength": 8.0}</t>
+        </is>
+      </c>
+      <c r="AC42" t="inlineStr">
+        <is>
+          <t>{"Consistency": 17.6, "Controversy": 2.9, "Dirtiness": 3.1, "Important Matches": 17.6, "Injury Proneness": 2.3, "Loyalty": 19.6, "Pressure": 17.1, "Professionalism": 18.0, "Sportsmanship": 19.6, "Temperament": 17.8, "Versatility": 3.8, "Ambition": 18.0, "Adaptability": 17.6}</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ollie  </t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Chessum  </t>
+        </is>
+      </c>
+      <c r="D43" s="2" t="n">
+        <v>32915</v>
+      </c>
+      <c r="E43" t="n">
+        <v>183</v>
+      </c>
+      <c r="F43" t="n">
+        <v>100</v>
+      </c>
+      <c r="G43" t="n">
+        <v>2</v>
+      </c>
+      <c r="H43" t="n">
+        <v>75</v>
+      </c>
+      <c r="I43" t="inlineStr"/>
+      <c r="J43" t="inlineStr"/>
+      <c r="K43" t="inlineStr"/>
+      <c r="L43" t="inlineStr"/>
+      <c r="M43" t="inlineStr"/>
+      <c r="N43" t="inlineStr">
+        <is>
+          <t>sr:5</t>
+        </is>
+      </c>
+      <c r="O43" t="n">
+        <v>4</v>
+      </c>
+      <c r="P43" t="inlineStr"/>
+      <c r="Q43" t="inlineStr"/>
+      <c r="R43" t="inlineStr"/>
+      <c r="S43" t="inlineStr"/>
+      <c r="T43" t="inlineStr"/>
+      <c r="U43" t="inlineStr"/>
+      <c r="V43" t="inlineStr"/>
+      <c r="W43" t="inlineStr"/>
+      <c r="X43" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y43" t="inlineStr"/>
+      <c r="Z43" t="inlineStr"/>
+      <c r="AA43" t="inlineStr"/>
+      <c r="AB43" t="inlineStr">
+        <is>
+          <t>{"darts": 4.0, "finishing": 10.0, "footwork": 8.0, "goal_kicking": 1.0, "handling": 18.0, "kicking": 2.0, "kicking_power": 2.0, "lineouts": 9.0, "marking": 9.0, "offloading": 16.0, "passing": 17.0, "scrummaging": 16.0, "rucking": 12.0, "technique": 15.0, "aggression": 5.0, "anticipation": 11.0, "bravery": 4.0, "composure": 4.0, "concentration": 18.0, "decisions": 18.0, "determination": 17.0, "flair": 9.0, "leadership": 18.0, "off_the_ball": 10.0, "positioning": 5.0, "teamwork": 15.0, "vision": 10.0, "work_rate": 13.0, "acceleration": 3.0, "agility": 13.0, "balance": 12.0, "jumping_reach": 6.0, "natural_fitness": 6.0, "pace": 9.0, "stamina": 19.0, "strength": 5.0}</t>
+        </is>
+      </c>
+      <c r="AC43" t="inlineStr">
+        <is>
+          <t>{"Consistency": 18.3, "Controversy": 3.1, "Dirtiness": 1.5, "Important Matches": 14.1, "Injury Proneness": 3.3, "Loyalty": 15.0, "Pressure": 15.8, "Professionalism": 18.2, "Sportsmanship": 18.7, "Temperament": 19.3, "Versatility": 4.8, "Ambition": 18.1, "Adaptability": 19.2}</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Chandler  </t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cunningham-South  </t>
+        </is>
+      </c>
+      <c r="D44" s="2" t="n">
+        <v>32916</v>
+      </c>
+      <c r="E44" t="n">
+        <v>183</v>
+      </c>
+      <c r="F44" t="n">
+        <v>100</v>
+      </c>
+      <c r="G44" t="n">
+        <v>2</v>
+      </c>
+      <c r="H44" t="n">
+        <v>75</v>
+      </c>
+      <c r="I44" t="inlineStr"/>
+      <c r="J44" t="inlineStr"/>
+      <c r="K44" t="inlineStr"/>
+      <c r="L44" t="inlineStr"/>
+      <c r="M44" t="inlineStr"/>
+      <c r="N44" t="inlineStr">
+        <is>
+          <t>br:5</t>
+        </is>
+      </c>
+      <c r="O44" t="n">
+        <v>5</v>
+      </c>
+      <c r="P44" t="inlineStr"/>
+      <c r="Q44" t="inlineStr"/>
+      <c r="R44" t="inlineStr"/>
+      <c r="S44" t="inlineStr"/>
+      <c r="T44" t="inlineStr"/>
+      <c r="U44" t="inlineStr"/>
+      <c r="V44" t="inlineStr"/>
+      <c r="W44" t="inlineStr"/>
+      <c r="X44" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y44" t="inlineStr"/>
+      <c r="Z44" t="inlineStr"/>
+      <c r="AA44" t="inlineStr"/>
+      <c r="AB44" t="inlineStr">
+        <is>
+          <t>{"darts": 3.0, "finishing": 11.0, "footwork": 15.0, "goal_kicking": 3.0, "handling": 16.0, "kicking": 12.0, "kicking_power": 9.0, "lineouts": 4.0, "marking": 2.0, "offloading": 18.0, "passing": 19.0, "scrummaging": 2.0, "rucking": 7.0, "technique": 18.0, "aggression": 7.0, "anticipation": 8.0, "bravery": 14.0, "composure": 20.0, "concentration": 8.0, "decisions": 7.0, "determination": 9.0, "flair": 10.0, "leadership": 8.0, "off_the_ball": 7.0, "positioning": 11.0, "teamwork": 10.0, "vision": 4.0, "work_rate": 8.0, "acceleration": 14.0, "agility": 15.0, "balance": 5.0, "jumping_reach": 17.0, "natural_fitness": 13.0, "pace": 18.0, "stamina": 15.0, "strength": 11.0}</t>
+        </is>
+      </c>
+      <c r="AC44" t="inlineStr">
+        <is>
+          <t>{"Consistency": 14.4, "Controversy": 1.6, "Dirtiness": 1.2, "Important Matches": 14.1, "Injury Proneness": 5.1, "Loyalty": 19.3, "Pressure": 17.5, "Professionalism": 19.8, "Sportsmanship": 19.3, "Temperament": 17.4, "Versatility": 6.0, "Ambition": 19.4, "Adaptability": 19.1}</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Harry  </t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Randall  </t>
+        </is>
+      </c>
+      <c r="D45" s="2" t="n">
+        <v>32917</v>
+      </c>
+      <c r="E45" t="n">
+        <v>183</v>
+      </c>
+      <c r="F45" t="n">
+        <v>100</v>
+      </c>
+      <c r="G45" t="n">
+        <v>2</v>
+      </c>
+      <c r="H45" t="n">
+        <v>75</v>
+      </c>
+      <c r="I45" t="inlineStr"/>
+      <c r="J45" t="inlineStr"/>
+      <c r="K45" t="inlineStr"/>
+      <c r="L45" t="inlineStr"/>
+      <c r="M45" t="inlineStr"/>
+      <c r="N45" t="inlineStr">
+        <is>
+          <t>sh:5</t>
+        </is>
+      </c>
+      <c r="O45" t="n">
+        <v>6</v>
+      </c>
+      <c r="P45" t="inlineStr"/>
+      <c r="Q45" t="inlineStr"/>
+      <c r="R45" t="inlineStr"/>
+      <c r="S45" t="inlineStr"/>
+      <c r="T45" t="inlineStr"/>
+      <c r="U45" t="inlineStr"/>
+      <c r="V45" t="inlineStr"/>
+      <c r="W45" t="inlineStr"/>
+      <c r="X45" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y45" t="inlineStr"/>
+      <c r="Z45" t="inlineStr"/>
+      <c r="AA45" t="inlineStr"/>
+      <c r="AB45" t="inlineStr">
+        <is>
+          <t>{"darts": 2.0, "finishing": 11.0, "footwork": 4.0, "goal_kicking": 18.0, "handling": 18.0, "kicking": 6.0, "kicking_power": 18.0, "lineouts": 6.0, "marking": 5.0, "offloading": 18.0, "passing": 14.0, "scrummaging": 17.0, "rucking": 17.0, "technique": 9.0, "aggression": 3.0, "anticipation": 7.0, "bravery": 13.0, "composure": 4.0, "concentration": 14.0, "decisions": 7.0, "determination": 5.0, "flair": 1.0, "leadership": 16.0, "off_the_ball": 2.0, "positioning": 13.0, "teamwork": 10.0, "vision": 10.0, "work_rate": 11.0, "acceleration": 15.0, "agility": 5.0, "balance": 16.0, "jumping_reach": 2.0, "natural_fitness": 17.0, "pace": 7.0, "stamina": 4.0, "strength": 19.0}</t>
+        </is>
+      </c>
+      <c r="AC45" t="inlineStr">
+        <is>
+          <t>{"Consistency": 17.7, "Controversy": 1.4, "Dirtiness": 3.9, "Important Matches": 18.9, "Injury Proneness": 4.8, "Loyalty": 16.8, "Pressure": 18.9, "Professionalism": 19.1, "Sportsmanship": 19.7, "Temperament": 19.6, "Versatility": 14.8, "Ambition": 17.6, "Adaptability": 18.0}</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Fin</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Smith</t>
+        </is>
+      </c>
+      <c r="D46" s="2" t="n">
+        <v>32918</v>
+      </c>
+      <c r="E46" t="n">
+        <v>183</v>
+      </c>
+      <c r="F46" t="n">
+        <v>100</v>
+      </c>
+      <c r="G46" t="n">
+        <v>2</v>
+      </c>
+      <c r="H46" t="n">
+        <v>75</v>
+      </c>
+      <c r="I46" t="inlineStr"/>
+      <c r="J46" t="inlineStr"/>
+      <c r="K46" t="inlineStr"/>
+      <c r="L46" t="inlineStr"/>
+      <c r="M46" t="inlineStr"/>
+      <c r="N46" t="inlineStr">
+        <is>
+          <t>fh:5</t>
+        </is>
+      </c>
+      <c r="O46" t="n">
+        <v>7</v>
+      </c>
+      <c r="P46" t="inlineStr"/>
+      <c r="Q46" t="inlineStr"/>
+      <c r="R46" t="inlineStr"/>
+      <c r="S46" t="inlineStr"/>
+      <c r="T46" t="inlineStr"/>
+      <c r="U46" t="inlineStr"/>
+      <c r="V46" t="inlineStr"/>
+      <c r="W46" t="inlineStr"/>
+      <c r="X46" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y46" t="inlineStr"/>
+      <c r="Z46" t="inlineStr"/>
+      <c r="AA46" t="inlineStr"/>
+      <c r="AB46" t="inlineStr">
+        <is>
+          <t>{"darts": 4.0, "finishing": 7.0, "footwork": 12.0, "goal_kicking": 14.0, "handling": 9.0, "kicking": 7.0, "kicking_power": 15.0, "lineouts": 7.0, "marking": 15.0, "offloading": 3.0, "passing": 6.0, "scrummaging": 19.0, "rucking": 7.0, "technique": 4.0, "aggression": 6.0, "anticipation": 3.0, "bravery": 20.0, "composure": 19.0, "concentration": 4.0, "decisions": 9.0, "determination": 14.0, "flair": 13.0, "leadership": 16.0, "off_the_ball": 8.0, "positioning": 7.0, "teamwork": 4.0, "vision": 3.0, "work_rate": 9.0, "acceleration": 16.0, "agility": 4.0, "balance": 3.0, "jumping_reach": 20.0, "natural_fitness": 10.0, "pace": 13.0, "stamina": 19.0, "strength": 7.0}</t>
+        </is>
+      </c>
+      <c r="AC46" t="inlineStr">
+        <is>
+          <t>{"Consistency": 14.9, "Controversy": 2.4, "Dirtiness": 3.6, "Important Matches": 18.1, "Injury Proneness": 3.7, "Loyalty": 14.0, "Pressure": 14.8, "Professionalism": 19.0, "Sportsmanship": 19.7, "Temperament": 19.7, "Versatility": 9.2, "Ambition": 19.2, "Adaptability": 17.4}</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Will  </t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Muir</t>
+        </is>
+      </c>
+      <c r="D47" s="2" t="n">
+        <v>32919</v>
+      </c>
+      <c r="E47" t="n">
+        <v>183</v>
+      </c>
+      <c r="F47" t="n">
+        <v>100</v>
+      </c>
+      <c r="G47" t="n">
+        <v>2</v>
+      </c>
+      <c r="H47" t="n">
+        <v>75</v>
+      </c>
+      <c r="I47" t="inlineStr"/>
+      <c r="J47" t="inlineStr"/>
+      <c r="K47" t="inlineStr"/>
+      <c r="L47" t="inlineStr"/>
+      <c r="M47" t="inlineStr"/>
+      <c r="N47" t="inlineStr">
+        <is>
+          <t>wg:5</t>
+        </is>
+      </c>
+      <c r="O47" t="n">
+        <v>9</v>
+      </c>
+      <c r="P47" t="inlineStr"/>
+      <c r="Q47" t="inlineStr"/>
+      <c r="R47" t="inlineStr"/>
+      <c r="S47" t="inlineStr"/>
+      <c r="T47" t="inlineStr"/>
+      <c r="U47" t="inlineStr"/>
+      <c r="V47" t="inlineStr"/>
+      <c r="W47" t="inlineStr"/>
+      <c r="X47" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y47" t="inlineStr"/>
+      <c r="Z47" t="inlineStr"/>
+      <c r="AA47" t="inlineStr"/>
+      <c r="AB47" t="inlineStr">
+        <is>
+          <t>{"darts": 4.0, "finishing": 14.0, "footwork": 11.0, "goal_kicking": 17.0, "handling": 19.0, "kicking": 3.0, "kicking_power": 11.0, "lineouts": 5.0, "marking": 20.0, "offloading": 4.0, "passing": 4.0, "scrummaging": 19.0, "rucking": 17.0, "technique": 6.0, "aggression": 17.0, "anticipation": 15.0, "bravery": 1.0, "composure": 18.0, "concentration": 17.0, "decisions": 4.0, "determination": 8.0, "flair": 4.0, "leadership": 11.0, "off_the_ball": 6.0, "positioning": 7.0, "teamwork": 8.0, "vision": 4.0, "work_rate": 11.0, "acceleration": 9.0, "agility": 12.0, "balance": 2.0, "jumping_reach": 9.0, "natural_fitness": 4.0, "pace": 16.0, "stamina": 12.0, "strength": 9.0}</t>
+        </is>
+      </c>
+      <c r="AC47" t="inlineStr">
+        <is>
+          <t>{"Consistency": 17.9, "Controversy": 1.3, "Dirtiness": 4.2, "Important Matches": 18.0, "Injury Proneness": 15.8, "Loyalty": 15.0, "Pressure": 18.5, "Professionalism": 19.1, "Sportsmanship": 18.7, "Temperament": 18.1, "Versatility": 4.1, "Ambition": 18.9, "Adaptability": 18.4}</t>
         </is>
       </c>
     </row>

</xml_diff>